<commit_message>
Added more info to the data table in the home page
</commit_message>
<xml_diff>
--- a/input/Rivals of Aether Academy Frame Data - Updated for 2.0.7.0.xlsx
+++ b/input/Rivals of Aether Academy Frame Data - Updated for 2.0.7.0.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" state="visible" r:id="rId2"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6742" uniqueCount="1740">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6751" uniqueCount="1740">
   <si>
     <r>
       <rPr>
@@ -2168,7 +2168,7 @@
     <t xml:space="preserve">Neutral Special: Explosion</t>
   </si>
   <si>
-    <t xml:space="preserve">Forward Special: Uncharged Missile</t>
+    <t xml:space="preserve">Forward Special: Uncharged Missile (Least travel time)</t>
   </si>
   <si>
     <t xml:space="preserve">9-42 (Charge startup)
@@ -2182,13 +2182,13 @@
 61 (Maximum)</t>
   </si>
   <si>
-    <t xml:space="preserve">2-5 (Gains 1 damage every 60 frames of travel to a max of 5)</t>
-  </si>
-  <si>
     <t xml:space="preserve">20 (Applied on Last Frame of Endlag)</t>
   </si>
   <si>
     <t xml:space="preserve">You lose control over the missile on death. Can not trigger galaxy kill effect on a character who is stuck by a mine. Missiles have a base damage of 2%, but will increase by 1% every 60 frames of travel to deal a maximum of 5%. Missiles do not have an explosion hitbox, so a hidden pillar destruction hitbox will appear on missile exploding. The radius for this for uncharged missiles is 32 pixels.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forward Special: Uncharged Missile (Most travel time)</t>
   </si>
   <si>
     <t xml:space="preserve">Forward Special: Charged Missile</t>
@@ -2705,7 +2705,7 @@
     <t xml:space="preserve">An existing rock near Kragg will be picked up on f8, interrupting the active frames. Hitting Kragg anytime from f8- will cause him to be in hitstun with the rock in his hands. Inputting dodge during the first 5 frames of startup will prevent a nearby rock from being picked up and will perform rock shine as usual.</t>
   </si>
   <si>
-    <t xml:space="preserve">Rock: Shards</t>
+    <t xml:space="preserve">Neutral Special: Rock: (Shards)</t>
   </si>
   <si>
     <t xml:space="preserve">10 (Grounded rock) 
@@ -2719,19 +2719,19 @@
     <t xml:space="preserve">Breaking the rock has 10 frames hitpause, with 1 further frame of hitpause on breaking airborne rocks due to rock state change.</t>
   </si>
   <si>
-    <t xml:space="preserve">Rock: Neutral Throw</t>
+    <t xml:space="preserve">Neutral Special: Rock: (Neutral Throw)</t>
   </si>
   <si>
     <t xml:space="preserve">7-</t>
   </si>
   <si>
-    <t xml:space="preserve">Rock: Forward Throw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rock: Up Throw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rock: Down Throw</t>
+    <t xml:space="preserve">Neutral Special: Rock: (Forward Throw)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neutral Special: Rock (Up Throw)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neutral Special: Rock: (Down Throw)</t>
   </si>
   <si>
     <t xml:space="preserve">Forward Special: Ground</t>
@@ -7654,11 +7654,11 @@
   </sheetPr>
   <dimension ref="A1:Q44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="3.14"/>
@@ -8801,7 +8801,7 @@
   </sheetPr>
   <dimension ref="A1:AB44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -8809,7 +8809,7 @@
       <selection pane="bottomRight" activeCell="H33" activeCellId="0" sqref="H33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.57"/>
@@ -11551,13 +11551,13 @@
   </sheetPr>
   <dimension ref="A1:Z54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="D10" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
       <selection pane="topRight" activeCell="H53" activeCellId="0" sqref="H53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="42.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.98"/>
@@ -14609,7 +14609,7 @@
   </sheetPr>
   <dimension ref="A1:Y54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -14617,7 +14617,7 @@
       <selection pane="bottomRight" activeCell="H50" activeCellId="0" sqref="H50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.57"/>
@@ -17595,7 +17595,7 @@
   </sheetPr>
   <dimension ref="A1:AB75"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -17603,7 +17603,7 @@
       <selection pane="bottomRight" activeCell="H57" activeCellId="0" sqref="H57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.43"/>
@@ -21633,7 +21633,7 @@
   </sheetPr>
   <dimension ref="A1:AA1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -21641,7 +21641,7 @@
       <selection pane="bottomRight" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.71"/>
@@ -24884,7 +24884,7 @@
   </sheetPr>
   <dimension ref="A1:Y43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -24892,7 +24892,7 @@
       <selection pane="bottomRight" activeCell="L35" activeCellId="0" sqref="L35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="40.14"/>
@@ -27341,13 +27341,13 @@
   </sheetPr>
   <dimension ref="A1:Z45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.14"/>
@@ -29912,11 +29912,11 @@
   </sheetPr>
   <dimension ref="A1:AG30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="359" t="s">
@@ -30718,11 +30718,11 @@
   </sheetPr>
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="45" width="11.52"/>
   </cols>
@@ -30891,7 +30891,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
@@ -33564,7 +33564,7 @@
   </sheetPr>
   <dimension ref="A1:Y1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
@@ -33572,7 +33572,7 @@
       <selection pane="bottomRight" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="38.43"/>
@@ -37168,7 +37168,7 @@
   </sheetPr>
   <dimension ref="A1:AA57"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
@@ -37176,7 +37176,7 @@
       <selection pane="bottomRight" activeCell="L52" activeCellId="0" sqref="L52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="21.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="21.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.43"/>
@@ -40487,15 +40487,15 @@
   </sheetPr>
   <dimension ref="A1:AG1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="D16" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+      <selection pane="bottomRight" activeCell="I37" activeCellId="0" sqref="I37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25"/>
@@ -42554,8 +42554,8 @@
       <c r="F36" s="136" t="s">
         <v>659</v>
       </c>
-      <c r="G36" s="173" t="s">
-        <v>660</v>
+      <c r="G36" s="173" t="n">
+        <v>2</v>
       </c>
       <c r="H36" s="102" t="n">
         <v>50</v>
@@ -42575,7 +42575,7 @@
       <c r="M36" s="102"/>
       <c r="N36" s="102"/>
       <c r="O36" s="115" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="P36" s="102" t="n">
         <v>6</v>
@@ -42590,7 +42590,7 @@
         <v>129</v>
       </c>
       <c r="T36" s="137" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="U36" s="137"/>
       <c r="V36" s="137"/>
@@ -42600,415 +42600,476 @@
       <c r="Z36" s="137"/>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="162" t="s">
+      <c r="A37" s="102" t="s">
+        <v>662</v>
+      </c>
+      <c r="B37" s="136" t="s">
+        <v>657</v>
+      </c>
+      <c r="C37" s="98" t="s">
+        <v>658</v>
+      </c>
+      <c r="D37" s="98" t="s">
+        <v>464</v>
+      </c>
+      <c r="E37" s="98"/>
+      <c r="F37" s="136" t="s">
+        <v>659</v>
+      </c>
+      <c r="G37" s="173" t="n">
+        <v>5</v>
+      </c>
+      <c r="H37" s="102" t="n">
+        <v>50</v>
+      </c>
+      <c r="I37" s="102" t="n">
+        <v>7</v>
+      </c>
+      <c r="J37" s="98" t="s">
+        <v>323</v>
+      </c>
+      <c r="K37" s="102" t="n">
+        <v>3</v>
+      </c>
+      <c r="L37" s="102" t="s">
+        <v>156</v>
+      </c>
+      <c r="M37" s="102"/>
+      <c r="N37" s="102"/>
+      <c r="O37" s="115" t="s">
+        <v>660</v>
+      </c>
+      <c r="P37" s="102" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q37" s="102" t="n">
+        <v>0</v>
+      </c>
+      <c r="R37" s="102" t="n">
+        <v>0</v>
+      </c>
+      <c r="S37" s="102" t="s">
+        <v>129</v>
+      </c>
+      <c r="T37" s="137" t="s">
+        <v>661</v>
+      </c>
+      <c r="U37" s="137"/>
+      <c r="V37" s="137"/>
+      <c r="W37" s="137"/>
+      <c r="X37" s="137"/>
+      <c r="Y37" s="137"/>
+      <c r="Z37" s="137"/>
+    </row>
+    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="162" t="s">
         <v>663</v>
       </c>
-      <c r="B37" s="178" t="s">
+      <c r="B38" s="178" t="s">
         <v>664</v>
       </c>
-      <c r="C37" s="163" t="s">
+      <c r="C38" s="163" t="s">
         <v>665</v>
       </c>
-      <c r="D37" s="163" t="s">
+      <c r="D38" s="163" t="s">
         <v>148</v>
       </c>
-      <c r="E37" s="163"/>
-      <c r="F37" s="163" t="s">
+      <c r="E38" s="163"/>
+      <c r="F38" s="163" t="s">
         <v>666</v>
       </c>
-      <c r="G37" s="162" t="n">
+      <c r="G38" s="162" t="n">
         <v>20</v>
       </c>
-      <c r="H37" s="162" t="n">
+      <c r="H38" s="162" t="n">
         <v>40</v>
       </c>
-      <c r="I37" s="162" t="n">
+      <c r="I38" s="162" t="n">
         <v>6</v>
       </c>
-      <c r="J37" s="163" t="s">
+      <c r="J38" s="163" t="s">
         <v>216</v>
       </c>
-      <c r="K37" s="162" t="n">
+      <c r="K38" s="162" t="n">
         <v>3</v>
       </c>
-      <c r="L37" s="162" t="s">
+      <c r="L38" s="162" t="s">
         <v>156</v>
       </c>
-      <c r="M37" s="162"/>
-      <c r="N37" s="162"/>
-      <c r="O37" s="162"/>
-      <c r="P37" s="162" t="n">
+      <c r="M38" s="162"/>
+      <c r="N38" s="162"/>
+      <c r="O38" s="162"/>
+      <c r="P38" s="162" t="n">
         <v>10</v>
       </c>
-      <c r="Q37" s="162" t="n">
+      <c r="Q38" s="162" t="n">
         <v>90</v>
       </c>
-      <c r="R37" s="162" t="n">
-        <v>0</v>
-      </c>
-      <c r="S37" s="162" t="s">
-        <v>129</v>
-      </c>
-      <c r="T37" s="166" t="s">
+      <c r="R38" s="162" t="n">
+        <v>0</v>
+      </c>
+      <c r="S38" s="162" t="s">
+        <v>129</v>
+      </c>
+      <c r="T38" s="166" t="s">
         <v>667</v>
       </c>
-      <c r="U37" s="166"/>
-      <c r="V37" s="166"/>
-      <c r="W37" s="166"/>
-      <c r="X37" s="166"/>
-      <c r="Y37" s="166"/>
-      <c r="Z37" s="166"/>
-    </row>
-    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="102" t="s">
+      <c r="U38" s="166"/>
+      <c r="V38" s="166"/>
+      <c r="W38" s="166"/>
+      <c r="X38" s="166"/>
+      <c r="Y38" s="166"/>
+      <c r="Z38" s="166"/>
+    </row>
+    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="102" t="s">
         <v>668</v>
       </c>
-      <c r="B38" s="98"/>
-      <c r="C38" s="136" t="s">
+      <c r="B39" s="98"/>
+      <c r="C39" s="136" t="s">
         <v>669</v>
       </c>
-      <c r="D38" s="98"/>
-      <c r="E38" s="98"/>
-      <c r="F38" s="98"/>
-      <c r="G38" s="102"/>
-      <c r="H38" s="102"/>
-      <c r="I38" s="102"/>
-      <c r="J38" s="98"/>
-      <c r="K38" s="102"/>
-      <c r="L38" s="102"/>
-      <c r="M38" s="102"/>
-      <c r="N38" s="102"/>
-      <c r="O38" s="102"/>
-      <c r="P38" s="102"/>
-      <c r="Q38" s="102"/>
-      <c r="R38" s="102"/>
-      <c r="S38" s="102"/>
-      <c r="T38" s="137" t="s">
+      <c r="D39" s="98"/>
+      <c r="E39" s="98"/>
+      <c r="F39" s="98"/>
+      <c r="G39" s="102"/>
+      <c r="H39" s="102"/>
+      <c r="I39" s="102"/>
+      <c r="J39" s="98"/>
+      <c r="K39" s="102"/>
+      <c r="L39" s="102"/>
+      <c r="M39" s="102"/>
+      <c r="N39" s="102"/>
+      <c r="O39" s="102"/>
+      <c r="P39" s="102"/>
+      <c r="Q39" s="102"/>
+      <c r="R39" s="102"/>
+      <c r="S39" s="102"/>
+      <c r="T39" s="137" t="s">
         <v>670</v>
       </c>
-      <c r="U38" s="137"/>
-      <c r="V38" s="137"/>
-      <c r="W38" s="137"/>
-      <c r="X38" s="137"/>
-      <c r="Y38" s="137"/>
-      <c r="Z38" s="137"/>
-    </row>
-    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="162" t="s">
+      <c r="U39" s="137"/>
+      <c r="V39" s="137"/>
+      <c r="W39" s="137"/>
+      <c r="X39" s="137"/>
+      <c r="Y39" s="137"/>
+      <c r="Z39" s="137"/>
+    </row>
+    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="162" t="s">
         <v>671</v>
       </c>
-      <c r="B39" s="165" t="s">
+      <c r="B40" s="165" t="s">
         <v>672</v>
       </c>
-      <c r="C39" s="165" t="s">
+      <c r="C40" s="165" t="s">
         <v>673</v>
       </c>
-      <c r="D39" s="163"/>
-      <c r="E39" s="163"/>
-      <c r="F39" s="163"/>
-      <c r="G39" s="162" t="n">
+      <c r="D40" s="163"/>
+      <c r="E40" s="163"/>
+      <c r="F40" s="163"/>
+      <c r="G40" s="162" t="n">
         <v>10</v>
       </c>
-      <c r="H39" s="162" t="n">
+      <c r="H40" s="162" t="n">
         <v>70</v>
       </c>
-      <c r="I39" s="162" t="n">
+      <c r="I40" s="162" t="n">
         <v>10</v>
       </c>
-      <c r="J39" s="163" t="s">
+      <c r="J40" s="163" t="s">
         <v>181</v>
       </c>
-      <c r="K39" s="162" t="n">
+      <c r="K40" s="162" t="n">
         <v>10</v>
       </c>
-      <c r="L39" s="162" t="s">
+      <c r="L40" s="162" t="s">
         <v>128</v>
       </c>
-      <c r="M39" s="162"/>
-      <c r="N39" s="162"/>
-      <c r="O39" s="162"/>
-      <c r="P39" s="162" t="n">
+      <c r="M40" s="162"/>
+      <c r="N40" s="162"/>
+      <c r="O40" s="162"/>
+      <c r="P40" s="162" t="n">
         <v>10</v>
       </c>
-      <c r="Q39" s="162" t="n">
+      <c r="Q40" s="162" t="n">
         <v>80</v>
       </c>
-      <c r="R39" s="162" t="n">
+      <c r="R40" s="162" t="n">
         <v>3</v>
       </c>
-      <c r="S39" s="162" t="s">
-        <v>129</v>
-      </c>
-      <c r="T39" s="168" t="s">
+      <c r="S40" s="162" t="s">
+        <v>129</v>
+      </c>
+      <c r="T40" s="168" t="s">
         <v>674</v>
       </c>
-      <c r="U39" s="168"/>
-      <c r="V39" s="168"/>
-      <c r="W39" s="168"/>
-      <c r="X39" s="168"/>
-      <c r="Y39" s="168"/>
-      <c r="Z39" s="168"/>
-    </row>
-    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="102" t="s">
+      <c r="U40" s="168"/>
+      <c r="V40" s="168"/>
+      <c r="W40" s="168"/>
+      <c r="X40" s="168"/>
+      <c r="Y40" s="168"/>
+      <c r="Z40" s="168"/>
+    </row>
+    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="102" t="s">
         <v>675</v>
       </c>
-      <c r="B40" s="98"/>
-      <c r="C40" s="136" t="s">
+      <c r="B41" s="98"/>
+      <c r="C41" s="136" t="s">
         <v>676</v>
       </c>
-      <c r="D40" s="98" t="s">
+      <c r="D41" s="98" t="s">
         <v>135</v>
       </c>
-      <c r="E40" s="98"/>
-      <c r="F40" s="98" t="s">
+      <c r="E41" s="98"/>
+      <c r="F41" s="98" t="s">
         <v>215</v>
       </c>
-      <c r="G40" s="102"/>
-      <c r="H40" s="102"/>
-      <c r="I40" s="102"/>
-      <c r="J40" s="98"/>
-      <c r="K40" s="102"/>
-      <c r="L40" s="102"/>
-      <c r="M40" s="102"/>
-      <c r="N40" s="102"/>
-      <c r="O40" s="102"/>
-      <c r="P40" s="102"/>
-      <c r="Q40" s="102"/>
-      <c r="R40" s="102"/>
-      <c r="S40" s="102"/>
-      <c r="T40" s="167" t="s">
+      <c r="G41" s="102"/>
+      <c r="H41" s="102"/>
+      <c r="I41" s="102"/>
+      <c r="J41" s="98"/>
+      <c r="K41" s="102"/>
+      <c r="L41" s="102"/>
+      <c r="M41" s="102"/>
+      <c r="N41" s="102"/>
+      <c r="O41" s="102"/>
+      <c r="P41" s="102"/>
+      <c r="Q41" s="102"/>
+      <c r="R41" s="102"/>
+      <c r="S41" s="102"/>
+      <c r="T41" s="167" t="s">
         <v>677</v>
       </c>
-      <c r="U40" s="167"/>
-      <c r="V40" s="167"/>
-      <c r="W40" s="167"/>
-      <c r="X40" s="167"/>
-      <c r="Y40" s="167"/>
-      <c r="Z40" s="167"/>
-    </row>
-    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="162" t="s">
+      <c r="U41" s="167"/>
+      <c r="V41" s="167"/>
+      <c r="W41" s="167"/>
+      <c r="X41" s="167"/>
+      <c r="Y41" s="167"/>
+      <c r="Z41" s="167"/>
+    </row>
+    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="162" t="s">
         <v>678</v>
       </c>
-      <c r="B41" s="163" t="s">
+      <c r="B42" s="163" t="s">
         <v>299</v>
       </c>
-      <c r="C41" s="179" t="s">
+      <c r="C42" s="179" t="s">
         <v>679</v>
       </c>
-      <c r="D41" s="163" t="s">
+      <c r="D42" s="163" t="s">
         <v>159</v>
       </c>
-      <c r="E41" s="163"/>
-      <c r="F41" s="162" t="n">
+      <c r="E42" s="163"/>
+      <c r="F42" s="162" t="n">
         <v>15</v>
       </c>
-      <c r="G41" s="162"/>
-      <c r="H41" s="162"/>
-      <c r="I41" s="162"/>
-      <c r="J41" s="163"/>
-      <c r="K41" s="162"/>
-      <c r="L41" s="162"/>
-      <c r="M41" s="162"/>
-      <c r="N41" s="162"/>
-      <c r="O41" s="177" t="s">
+      <c r="G42" s="162"/>
+      <c r="H42" s="162"/>
+      <c r="I42" s="162"/>
+      <c r="J42" s="163"/>
+      <c r="K42" s="162"/>
+      <c r="L42" s="162"/>
+      <c r="M42" s="162"/>
+      <c r="N42" s="162"/>
+      <c r="O42" s="177" t="s">
         <v>680</v>
       </c>
-      <c r="P41" s="162"/>
-      <c r="Q41" s="162"/>
-      <c r="R41" s="162"/>
-      <c r="S41" s="162"/>
-      <c r="T41" s="180" t="s">
+      <c r="P42" s="162"/>
+      <c r="Q42" s="162"/>
+      <c r="R42" s="162"/>
+      <c r="S42" s="162"/>
+      <c r="T42" s="180" t="s">
         <v>681</v>
       </c>
-      <c r="U41" s="180"/>
-      <c r="V41" s="180"/>
-      <c r="W41" s="180"/>
-      <c r="X41" s="180"/>
-      <c r="Y41" s="180"/>
-      <c r="Z41" s="180"/>
-    </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="102" t="s">
+      <c r="U42" s="180"/>
+      <c r="V42" s="180"/>
+      <c r="W42" s="180"/>
+      <c r="X42" s="180"/>
+      <c r="Y42" s="180"/>
+      <c r="Z42" s="180"/>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="102" t="s">
         <v>682</v>
       </c>
-      <c r="B42" s="98"/>
-      <c r="C42" s="136" t="s">
+      <c r="B43" s="98"/>
+      <c r="C43" s="136" t="s">
         <v>683</v>
       </c>
-      <c r="D42" s="98"/>
-      <c r="E42" s="98"/>
-      <c r="F42" s="102"/>
-      <c r="G42" s="102" t="n">
+      <c r="D43" s="98"/>
+      <c r="E43" s="98"/>
+      <c r="F43" s="102"/>
+      <c r="G43" s="102" t="n">
         <v>4</v>
       </c>
-      <c r="H42" s="102" t="n">
+      <c r="H43" s="102" t="n">
         <v>90</v>
       </c>
-      <c r="I42" s="102" t="n">
+      <c r="I43" s="102" t="n">
         <v>3</v>
       </c>
-      <c r="J42" s="98" t="s">
+      <c r="J43" s="98" t="s">
         <v>127</v>
       </c>
-      <c r="K42" s="102" t="n">
+      <c r="K43" s="102" t="n">
         <v>7</v>
       </c>
-      <c r="L42" s="102" t="s">
+      <c r="L43" s="102" t="s">
         <v>128</v>
       </c>
-      <c r="M42" s="102"/>
-      <c r="N42" s="102"/>
-      <c r="O42" s="102"/>
-      <c r="P42" s="102" t="n">
+      <c r="M43" s="102"/>
+      <c r="N43" s="102"/>
+      <c r="O43" s="102"/>
+      <c r="P43" s="102" t="n">
         <v>9</v>
       </c>
-      <c r="Q42" s="102" t="n">
-        <v>0</v>
-      </c>
-      <c r="R42" s="102" t="n">
+      <c r="Q43" s="102" t="n">
+        <v>0</v>
+      </c>
+      <c r="R43" s="102" t="n">
         <v>3</v>
       </c>
-      <c r="S42" s="102" t="s">
-        <v>129</v>
-      </c>
-      <c r="T42" s="132"/>
-      <c r="U42" s="132"/>
-      <c r="V42" s="132"/>
-      <c r="W42" s="132"/>
-      <c r="X42" s="132"/>
-      <c r="Y42" s="132"/>
-      <c r="Z42" s="132"/>
-    </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="162" t="s">
+      <c r="S43" s="102" t="s">
+        <v>129</v>
+      </c>
+      <c r="T43" s="132"/>
+      <c r="U43" s="132"/>
+      <c r="V43" s="132"/>
+      <c r="W43" s="132"/>
+      <c r="X43" s="132"/>
+      <c r="Y43" s="132"/>
+      <c r="Z43" s="132"/>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="162" t="s">
         <v>684</v>
       </c>
-      <c r="B43" s="163"/>
-      <c r="C43" s="162" t="s">
+      <c r="B44" s="163"/>
+      <c r="C44" s="162" t="s">
         <v>685</v>
       </c>
-      <c r="D43" s="163"/>
-      <c r="E43" s="163"/>
-      <c r="F43" s="162"/>
-      <c r="G43" s="162" t="n">
+      <c r="D44" s="163"/>
+      <c r="E44" s="163"/>
+      <c r="F44" s="162"/>
+      <c r="G44" s="162" t="n">
         <v>4</v>
       </c>
-      <c r="H43" s="162" t="n">
+      <c r="H44" s="162" t="n">
         <v>90</v>
       </c>
-      <c r="I43" s="162" t="n">
+      <c r="I44" s="162" t="n">
         <v>3</v>
       </c>
-      <c r="J43" s="163" t="s">
+      <c r="J44" s="163" t="s">
         <v>216</v>
       </c>
-      <c r="K43" s="162" t="n">
+      <c r="K44" s="162" t="n">
         <v>7</v>
       </c>
-      <c r="L43" s="162" t="s">
+      <c r="L44" s="162" t="s">
         <v>128</v>
       </c>
-      <c r="M43" s="162"/>
-      <c r="N43" s="162"/>
-      <c r="O43" s="162"/>
-      <c r="P43" s="162" t="n">
+      <c r="M44" s="162"/>
+      <c r="N44" s="162"/>
+      <c r="O44" s="162"/>
+      <c r="P44" s="162" t="n">
         <v>9</v>
       </c>
-      <c r="Q43" s="162" t="n">
-        <v>0</v>
-      </c>
-      <c r="R43" s="162" t="n">
+      <c r="Q44" s="162" t="n">
+        <v>0</v>
+      </c>
+      <c r="R44" s="162" t="n">
         <v>3</v>
       </c>
-      <c r="S43" s="162" t="s">
-        <v>129</v>
-      </c>
-      <c r="T43" s="164" t="s">
+      <c r="S44" s="162" t="s">
+        <v>129</v>
+      </c>
+      <c r="T44" s="164" t="s">
         <v>686</v>
       </c>
-      <c r="U43" s="164"/>
-      <c r="V43" s="164"/>
-      <c r="W43" s="164"/>
-      <c r="X43" s="164"/>
-      <c r="Y43" s="164"/>
-      <c r="Z43" s="164"/>
-    </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="102"/>
-      <c r="B44" s="102"/>
-      <c r="C44" s="102"/>
-      <c r="D44" s="102"/>
-      <c r="E44" s="102"/>
-      <c r="F44" s="102"/>
-      <c r="G44" s="102"/>
-      <c r="H44" s="102"/>
-      <c r="I44" s="102"/>
-      <c r="J44" s="102"/>
-      <c r="K44" s="102"/>
-      <c r="L44" s="102"/>
-      <c r="M44" s="102"/>
-      <c r="N44" s="102"/>
-      <c r="O44" s="102"/>
-      <c r="P44" s="102"/>
-      <c r="Q44" s="102"/>
-      <c r="R44" s="102"/>
-      <c r="S44" s="102"/>
-      <c r="T44" s="102"/>
-      <c r="U44" s="102"/>
-      <c r="V44" s="102"/>
-      <c r="W44" s="102"/>
-      <c r="X44" s="102"/>
-      <c r="Y44" s="102"/>
-    </row>
-    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="162"/>
-      <c r="K45" s="162"/>
-      <c r="L45" s="162"/>
-      <c r="M45" s="162"/>
-      <c r="N45" s="162"/>
-      <c r="O45" s="174"/>
-      <c r="P45" s="162"/>
-      <c r="Q45" s="162"/>
-      <c r="R45" s="162"/>
-      <c r="S45" s="162"/>
-      <c r="T45" s="162"/>
-      <c r="U45" s="162"/>
-      <c r="V45" s="162"/>
-      <c r="W45" s="162"/>
-      <c r="X45" s="162"/>
-      <c r="Y45" s="162"/>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T63" s="102"/>
-      <c r="U63" s="102"/>
-      <c r="V63" s="102"/>
-      <c r="W63" s="132"/>
-      <c r="X63" s="132"/>
-      <c r="Y63" s="132"/>
-      <c r="Z63" s="132"/>
-      <c r="AA63" s="132"/>
-      <c r="AB63" s="132"/>
-      <c r="AC63" s="132"/>
-      <c r="AD63" s="132"/>
-      <c r="AE63" s="132"/>
-      <c r="AF63" s="132"/>
-      <c r="AG63" s="132"/>
-    </row>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="U44" s="164"/>
+      <c r="V44" s="164"/>
+      <c r="W44" s="164"/>
+      <c r="X44" s="164"/>
+      <c r="Y44" s="164"/>
+      <c r="Z44" s="164"/>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="102"/>
+      <c r="B45" s="102"/>
+      <c r="C45" s="102"/>
+      <c r="D45" s="102"/>
+      <c r="E45" s="102"/>
+      <c r="F45" s="102"/>
+      <c r="G45" s="102"/>
+      <c r="H45" s="102"/>
+      <c r="I45" s="102"/>
+      <c r="J45" s="102"/>
+      <c r="K45" s="102"/>
+      <c r="L45" s="102"/>
+      <c r="M45" s="102"/>
+      <c r="N45" s="102"/>
+      <c r="O45" s="102"/>
+      <c r="P45" s="102"/>
+      <c r="Q45" s="102"/>
+      <c r="R45" s="102"/>
+      <c r="S45" s="102"/>
+      <c r="T45" s="102"/>
+      <c r="U45" s="102"/>
+      <c r="V45" s="102"/>
+      <c r="W45" s="102"/>
+      <c r="X45" s="102"/>
+      <c r="Y45" s="102"/>
+    </row>
+    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="162"/>
+      <c r="K46" s="162"/>
+      <c r="L46" s="162"/>
+      <c r="M46" s="162"/>
+      <c r="N46" s="162"/>
+      <c r="O46" s="174"/>
+      <c r="P46" s="162"/>
+      <c r="Q46" s="162"/>
+      <c r="R46" s="162"/>
+      <c r="S46" s="162"/>
+      <c r="T46" s="162"/>
+      <c r="U46" s="162"/>
+      <c r="V46" s="162"/>
+      <c r="W46" s="162"/>
+      <c r="X46" s="162"/>
+      <c r="Y46" s="162"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T64" s="102"/>
+      <c r="U64" s="102"/>
+      <c r="V64" s="102"/>
+      <c r="W64" s="132"/>
+      <c r="X64" s="132"/>
+      <c r="Y64" s="132"/>
+      <c r="Z64" s="132"/>
+      <c r="AA64" s="132"/>
+      <c r="AB64" s="132"/>
+      <c r="AC64" s="132"/>
+      <c r="AD64" s="132"/>
+      <c r="AE64" s="132"/>
+      <c r="AF64" s="132"/>
+      <c r="AG64" s="132"/>
+    </row>
     <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="43">
+  <mergeCells count="44">
     <mergeCell ref="T2:Z2"/>
     <mergeCell ref="T3:Z3"/>
     <mergeCell ref="T4:Z4"/>
@@ -43051,7 +43112,8 @@
     <mergeCell ref="T41:Z41"/>
     <mergeCell ref="T42:Z42"/>
     <mergeCell ref="T43:Z43"/>
-    <mergeCell ref="W63:AG63"/>
+    <mergeCell ref="T44:Z44"/>
+    <mergeCell ref="W64:AG64"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
@@ -43070,7 +43132,7 @@
   </sheetPr>
   <dimension ref="A1:AA1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="D14" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
@@ -43078,7 +43140,7 @@
       <selection pane="bottomRight" activeCell="K34" activeCellId="0" sqref="K34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.14"/>
@@ -45516,15 +45578,15 @@
   </sheetPr>
   <dimension ref="A1:AC41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O3" activeCellId="0" sqref="O3"/>
+      <selection pane="bottomRight" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="37.86"/>
@@ -48106,7 +48168,7 @@
   </sheetPr>
   <dimension ref="A1:Z33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -48114,7 +48176,7 @@
       <selection pane="bottomRight" activeCell="J37" activeCellId="0" sqref="J37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="43.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.29"/>

</xml_diff>

<commit_message>
Pushed new Zet fair and uair hitbox pics
</commit_message>
<xml_diff>
--- a/input/Rivals of Aether Academy Frame Data - Updated for 2.0.7.0.xlsx
+++ b/input/Rivals of Aether Academy Frame Data - Updated for 2.0.7.0.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" state="visible" r:id="rId2"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6751" uniqueCount="1740">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6753" uniqueCount="1740">
   <si>
     <r>
       <rPr>
@@ -4681,6 +4681,9 @@
     <t xml:space="preserve">Down Tilt Hit 1 (Sour)</t>
   </si>
   <si>
+    <t xml:space="preserve">10-11</t>
+  </si>
+  <si>
     <t xml:space="preserve">4 frames of extra hitpause on opponent.</t>
   </si>
   <si>
@@ -4988,9 +4991,6 @@
   </si>
   <si>
     <t xml:space="preserve">Fair Hit 2 (Late)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10-11</t>
   </si>
   <si>
     <t xml:space="preserve">28 (37 if grounded)</t>
@@ -5998,7 +5998,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="394">
+  <cellXfs count="393">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -7323,10 +7323,6 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="17" fillId="18" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="169" fontId="17" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -7658,7 +7654,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="3.14"/>
@@ -8802,14 +8798,14 @@
   <dimension ref="A1:AB44"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H33" activeCellId="0" sqref="H33"/>
+      <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="B29" activeCellId="0" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.57"/>
@@ -11557,7 +11553,7 @@
       <selection pane="topRight" activeCell="H53" activeCellId="0" sqref="H53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="42.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.98"/>
@@ -14617,7 +14613,7 @@
       <selection pane="bottomRight" activeCell="H50" activeCellId="0" sqref="H50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.57"/>
@@ -17603,7 +17599,7 @@
       <selection pane="bottomRight" activeCell="H57" activeCellId="0" sqref="H57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.43"/>
@@ -21638,10 +21634,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D17" activeCellId="0" sqref="D17"/>
+      <selection pane="bottomRight" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.71"/>
@@ -22463,8 +22459,8 @@
       <c r="B15" s="203" t="s">
         <v>161</v>
       </c>
-      <c r="C15" s="331" t="n">
-        <v>43414</v>
+      <c r="C15" s="331" t="s">
+        <v>1464</v>
       </c>
       <c r="D15" s="203" t="s">
         <v>464</v>
@@ -22510,7 +22506,7 @@
         <v>129</v>
       </c>
       <c r="T15" s="204" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="U15" s="204"/>
       <c r="V15" s="204"/>
@@ -22522,11 +22518,11 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="102" t="s">
-        <v>1465</v>
+        <v>1466</v>
       </c>
       <c r="B16" s="98"/>
-      <c r="C16" s="332" t="n">
-        <v>43414</v>
+      <c r="C16" s="331" t="s">
+        <v>1464</v>
       </c>
       <c r="D16" s="98"/>
       <c r="E16" s="98"/>
@@ -22567,7 +22563,7 @@
         <v>129</v>
       </c>
       <c r="T16" s="132" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="U16" s="132"/>
       <c r="V16" s="132"/>
@@ -22579,7 +22575,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="209" t="s">
-        <v>1466</v>
+        <v>1467</v>
       </c>
       <c r="B17" s="203"/>
       <c r="C17" s="209" t="s">
@@ -22632,7 +22628,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="102" t="s">
-        <v>1467</v>
+        <v>1468</v>
       </c>
       <c r="B18" s="98"/>
       <c r="C18" s="102" t="s">
@@ -22685,13 +22681,13 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="209" t="s">
-        <v>1468</v>
+        <v>1469</v>
       </c>
       <c r="B19" s="203" t="s">
         <v>464</v>
       </c>
       <c r="C19" s="203" t="s">
-        <v>1469</v>
+        <v>1470</v>
       </c>
       <c r="D19" s="203" t="s">
         <v>183</v>
@@ -22749,11 +22745,11 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="102" t="s">
-        <v>1470</v>
+        <v>1471</v>
       </c>
       <c r="B20" s="98"/>
       <c r="C20" s="98" t="s">
-        <v>1471</v>
+        <v>1472</v>
       </c>
       <c r="D20" s="98"/>
       <c r="E20" s="98"/>
@@ -22804,13 +22800,13 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="209" t="s">
-        <v>1472</v>
+        <v>1473</v>
       </c>
       <c r="B21" s="203" t="s">
         <v>170</v>
       </c>
       <c r="C21" s="203" t="s">
-        <v>1473</v>
+        <v>1474</v>
       </c>
       <c r="D21" s="203" t="n">
         <f aca="false">E21/3*2</f>
@@ -22835,7 +22831,7 @@
       <c r="J21" s="203" t="s">
         <v>216</v>
       </c>
-      <c r="K21" s="333" t="n">
+      <c r="K21" s="332" t="n">
         <v>43862</v>
       </c>
       <c r="L21" s="209" t="s">
@@ -22856,24 +22852,24 @@
       <c r="S21" s="209" t="s">
         <v>129</v>
       </c>
-      <c r="T21" s="334" t="s">
+      <c r="T21" s="333" t="s">
         <v>640</v>
       </c>
-      <c r="U21" s="334"/>
-      <c r="V21" s="334"/>
-      <c r="W21" s="334"/>
-      <c r="X21" s="334"/>
-      <c r="Y21" s="334"/>
-      <c r="Z21" s="334"/>
-      <c r="AA21" s="334"/>
+      <c r="U21" s="333"/>
+      <c r="V21" s="333"/>
+      <c r="W21" s="333"/>
+      <c r="X21" s="333"/>
+      <c r="Y21" s="333"/>
+      <c r="Z21" s="333"/>
+      <c r="AA21" s="333"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="102" t="s">
-        <v>1474</v>
+        <v>1475</v>
       </c>
       <c r="B22" s="98"/>
       <c r="C22" s="98" t="s">
-        <v>1473</v>
+        <v>1474</v>
       </c>
       <c r="D22" s="136"/>
       <c r="E22" s="136"/>
@@ -22890,7 +22886,7 @@
       <c r="J22" s="98" t="s">
         <v>308</v>
       </c>
-      <c r="K22" s="335" t="n">
+      <c r="K22" s="334" t="n">
         <v>43987</v>
       </c>
       <c r="L22" s="102" t="s">
@@ -22924,11 +22920,11 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="209" t="s">
-        <v>1475</v>
+        <v>1476</v>
       </c>
       <c r="B23" s="203"/>
       <c r="C23" s="203" t="s">
-        <v>1473</v>
+        <v>1474</v>
       </c>
       <c r="D23" s="203"/>
       <c r="E23" s="203"/>
@@ -22966,16 +22962,16 @@
       <c r="S23" s="209" t="s">
         <v>129</v>
       </c>
-      <c r="T23" s="334" t="s">
+      <c r="T23" s="333" t="s">
         <v>640</v>
       </c>
-      <c r="U23" s="334"/>
-      <c r="V23" s="334"/>
-      <c r="W23" s="334"/>
-      <c r="X23" s="334"/>
-      <c r="Y23" s="334"/>
-      <c r="Z23" s="334"/>
-      <c r="AA23" s="334"/>
+      <c r="U23" s="333"/>
+      <c r="V23" s="333"/>
+      <c r="W23" s="333"/>
+      <c r="X23" s="333"/>
+      <c r="Y23" s="333"/>
+      <c r="Z23" s="333"/>
+      <c r="AA23" s="333"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="102" t="s">
@@ -23050,7 +23046,7 @@
         <v>192</v>
       </c>
       <c r="C25" s="98" t="s">
-        <v>1476</v>
+        <v>1477</v>
       </c>
       <c r="D25" s="98" t="n">
         <f aca="false">E25/3*2</f>
@@ -23164,12 +23160,12 @@
       <c r="S26" s="209" t="s">
         <v>129</v>
       </c>
-      <c r="T26" s="334"/>
-      <c r="U26" s="334"/>
-      <c r="V26" s="334"/>
-      <c r="W26" s="334"/>
-      <c r="X26" s="334"/>
-      <c r="Y26" s="334"/>
+      <c r="T26" s="333"/>
+      <c r="U26" s="333"/>
+      <c r="V26" s="333"/>
+      <c r="W26" s="333"/>
+      <c r="X26" s="333"/>
+      <c r="Y26" s="333"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="102" t="s">
@@ -23224,7 +23220,7 @@
     </row>
     <row r="28" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="209" t="s">
-        <v>1477</v>
+        <v>1478</v>
       </c>
       <c r="B28" s="203" t="s">
         <v>183</v>
@@ -23280,7 +23276,7 @@
         <v>129</v>
       </c>
       <c r="T28" s="330" t="s">
-        <v>1478</v>
+        <v>1479</v>
       </c>
       <c r="U28" s="330"/>
       <c r="V28" s="330"/>
@@ -23290,7 +23286,7 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="102" t="s">
-        <v>1479</v>
+        <v>1480</v>
       </c>
       <c r="B29" s="98"/>
       <c r="C29" s="98" t="s">
@@ -23343,7 +23339,7 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="209" t="s">
-        <v>1480</v>
+        <v>1481</v>
       </c>
       <c r="B30" s="203"/>
       <c r="C30" s="203" t="s">
@@ -23385,18 +23381,18 @@
       <c r="S30" s="209" t="s">
         <v>129</v>
       </c>
-      <c r="T30" s="334" t="s">
+      <c r="T30" s="333" t="s">
         <v>640</v>
       </c>
-      <c r="U30" s="334"/>
-      <c r="V30" s="334"/>
-      <c r="W30" s="334"/>
-      <c r="X30" s="334"/>
-      <c r="Y30" s="334"/>
+      <c r="U30" s="333"/>
+      <c r="V30" s="333"/>
+      <c r="W30" s="333"/>
+      <c r="X30" s="333"/>
+      <c r="Y30" s="333"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="102" t="s">
-        <v>1481</v>
+        <v>1482</v>
       </c>
       <c r="B31" s="98"/>
       <c r="C31" s="98" t="s">
@@ -23449,7 +23445,7 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="209" t="s">
-        <v>1482</v>
+        <v>1483</v>
       </c>
       <c r="B32" s="203"/>
       <c r="C32" s="203" t="s">
@@ -23502,7 +23498,7 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="102" t="s">
-        <v>1483</v>
+        <v>1484</v>
       </c>
       <c r="B33" s="98"/>
       <c r="C33" s="98" t="s">
@@ -23555,17 +23551,17 @@
     </row>
     <row r="34" customFormat="false" ht="109.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="209" t="s">
-        <v>1484</v>
+        <v>1485</v>
       </c>
       <c r="B34" s="203"/>
       <c r="C34" s="202" t="s">
-        <v>1485</v>
+        <v>1486</v>
       </c>
       <c r="D34" s="203" t="s">
         <v>314</v>
       </c>
       <c r="E34" s="202" t="s">
-        <v>1486</v>
+        <v>1487</v>
       </c>
       <c r="F34" s="203"/>
       <c r="G34" s="209"/>
@@ -23582,7 +23578,7 @@
       <c r="R34" s="209"/>
       <c r="S34" s="209"/>
       <c r="T34" s="330" t="s">
-        <v>1487</v>
+        <v>1488</v>
       </c>
       <c r="U34" s="330"/>
       <c r="V34" s="330"/>
@@ -23626,7 +23622,7 @@
         <v>2</v>
       </c>
       <c r="L35" s="102" t="s">
-        <v>1488</v>
+        <v>1489</v>
       </c>
       <c r="M35" s="102" t="n">
         <v>8</v>
@@ -23698,18 +23694,18 @@
       <c r="S36" s="209" t="s">
         <v>129</v>
       </c>
-      <c r="T36" s="334" t="s">
+      <c r="T36" s="333" t="s">
         <v>723</v>
       </c>
-      <c r="U36" s="334"/>
-      <c r="V36" s="334"/>
-      <c r="W36" s="334"/>
-      <c r="X36" s="334"/>
-      <c r="Y36" s="334"/>
+      <c r="U36" s="333"/>
+      <c r="V36" s="333"/>
+      <c r="W36" s="333"/>
+      <c r="X36" s="333"/>
+      <c r="Y36" s="333"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="102" t="s">
-        <v>1489</v>
+        <v>1490</v>
       </c>
       <c r="B37" s="98" t="s">
         <v>192</v>
@@ -23766,7 +23762,7 @@
         <v>129</v>
       </c>
       <c r="T37" s="167" t="s">
-        <v>1490</v>
+        <v>1491</v>
       </c>
       <c r="U37" s="167"/>
       <c r="V37" s="167"/>
@@ -23776,11 +23772,11 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="209" t="s">
-        <v>1491</v>
+        <v>1492</v>
       </c>
       <c r="B38" s="203"/>
       <c r="C38" s="203" t="s">
-        <v>1492</v>
+        <v>1493</v>
       </c>
       <c r="G38" s="209" t="n">
         <v>7</v>
@@ -23815,16 +23811,16 @@
       <c r="S38" s="209" t="s">
         <v>129</v>
       </c>
-      <c r="T38" s="334"/>
-      <c r="U38" s="334"/>
-      <c r="V38" s="334"/>
-      <c r="W38" s="334"/>
-      <c r="X38" s="334"/>
-      <c r="Y38" s="334"/>
+      <c r="T38" s="333"/>
+      <c r="U38" s="333"/>
+      <c r="V38" s="333"/>
+      <c r="W38" s="333"/>
+      <c r="X38" s="333"/>
+      <c r="Y38" s="333"/>
     </row>
     <row r="39" customFormat="false" ht="25.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="102" t="s">
-        <v>1493</v>
+        <v>1494</v>
       </c>
       <c r="B39" s="98" t="s">
         <v>161</v>
@@ -23860,7 +23856,7 @@
       <c r="M39" s="102"/>
       <c r="N39" s="102"/>
       <c r="O39" s="102" t="s">
-        <v>1494</v>
+        <v>1495</v>
       </c>
       <c r="P39" s="102" t="n">
         <v>6</v>
@@ -23875,7 +23871,7 @@
         <v>129</v>
       </c>
       <c r="T39" s="167" t="s">
-        <v>1495</v>
+        <v>1496</v>
       </c>
       <c r="U39" s="167"/>
       <c r="V39" s="167"/>
@@ -23887,13 +23883,13 @@
     </row>
     <row r="40" customFormat="false" ht="14.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="209" t="s">
-        <v>1496</v>
+        <v>1497</v>
       </c>
       <c r="B40" s="203" t="s">
-        <v>1497</v>
+        <v>1498</v>
       </c>
       <c r="C40" s="203" t="s">
-        <v>1498</v>
+        <v>1499</v>
       </c>
       <c r="D40" s="203"/>
       <c r="E40" s="203"/>
@@ -23932,7 +23928,7 @@
         <v>129</v>
       </c>
       <c r="T40" s="212" t="s">
-        <v>1499</v>
+        <v>1500</v>
       </c>
       <c r="U40" s="212"/>
       <c r="V40" s="212"/>
@@ -23944,11 +23940,11 @@
     </row>
     <row r="41" customFormat="false" ht="89.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="102" t="s">
-        <v>1500</v>
+        <v>1501</v>
       </c>
       <c r="B41" s="98"/>
       <c r="C41" s="136" t="s">
-        <v>1501</v>
+        <v>1502</v>
       </c>
       <c r="D41" s="98"/>
       <c r="E41" s="98"/>
@@ -23967,7 +23963,7 @@
       <c r="R41" s="102"/>
       <c r="S41" s="102"/>
       <c r="T41" s="137" t="s">
-        <v>1502</v>
+        <v>1503</v>
       </c>
       <c r="U41" s="137"/>
       <c r="V41" s="137"/>
@@ -23982,17 +23978,17 @@
         <v>387</v>
       </c>
       <c r="B42" s="203" t="s">
-        <v>1503</v>
+        <v>1504</v>
       </c>
       <c r="C42" s="202" t="s">
-        <v>1504</v>
+        <v>1505</v>
       </c>
       <c r="D42" s="202" t="s">
         <v>148</v>
       </c>
       <c r="E42" s="202"/>
       <c r="F42" s="202" t="s">
-        <v>1505</v>
+        <v>1506</v>
       </c>
       <c r="G42" s="209" t="n">
         <v>8</v>
@@ -24028,7 +24024,7 @@
         <v>275</v>
       </c>
       <c r="T42" s="330" t="s">
-        <v>1506</v>
+        <v>1507</v>
       </c>
       <c r="U42" s="330"/>
       <c r="V42" s="330"/>
@@ -24040,20 +24036,20 @@
     </row>
     <row r="43" customFormat="false" ht="49.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="102" t="s">
-        <v>1507</v>
+        <v>1508</v>
       </c>
       <c r="B43" s="98" t="s">
         <v>192</v>
       </c>
       <c r="C43" s="98" t="s">
-        <v>1508</v>
+        <v>1509</v>
       </c>
       <c r="D43" s="98" t="s">
-        <v>1509</v>
+        <v>1510</v>
       </c>
       <c r="E43" s="98"/>
       <c r="F43" s="136" t="s">
-        <v>1510</v>
+        <v>1511</v>
       </c>
       <c r="G43" s="102" t="n">
         <v>2</v>
@@ -24101,7 +24097,7 @@
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="209" t="s">
-        <v>1511</v>
+        <v>1512</v>
       </c>
       <c r="B44" s="203"/>
       <c r="C44" s="203" t="s">
@@ -24156,7 +24152,7 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="102" t="s">
-        <v>1512</v>
+        <v>1513</v>
       </c>
       <c r="B45" s="98"/>
       <c r="C45" s="98" t="s">
@@ -24211,11 +24207,11 @@
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="209" t="s">
-        <v>1513</v>
+        <v>1514</v>
       </c>
       <c r="B46" s="203"/>
       <c r="C46" s="203" t="s">
-        <v>1514</v>
+        <v>1515</v>
       </c>
       <c r="D46" s="203"/>
       <c r="E46" s="203"/>
@@ -24266,11 +24262,11 @@
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="102" t="s">
-        <v>1515</v>
+        <v>1516</v>
       </c>
       <c r="B47" s="98"/>
       <c r="C47" s="98" t="s">
-        <v>1516</v>
+        <v>1517</v>
       </c>
       <c r="D47" s="98"/>
       <c r="E47" s="98"/>
@@ -24321,11 +24317,11 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="209" t="s">
-        <v>1517</v>
+        <v>1518</v>
       </c>
       <c r="B48" s="203"/>
       <c r="C48" s="203" t="s">
-        <v>1518</v>
+        <v>1519</v>
       </c>
       <c r="D48" s="203"/>
       <c r="E48" s="203"/>
@@ -24364,7 +24360,7 @@
         <v>275</v>
       </c>
       <c r="T48" s="204" t="s">
-        <v>1519</v>
+        <v>1520</v>
       </c>
       <c r="U48" s="204"/>
       <c r="V48" s="204"/>
@@ -24376,13 +24372,13 @@
     </row>
     <row r="49" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="102" t="s">
-        <v>1520</v>
+        <v>1521</v>
       </c>
       <c r="B49" s="136" t="s">
-        <v>1521</v>
+        <v>1522</v>
       </c>
       <c r="C49" s="98" t="s">
-        <v>1522</v>
+        <v>1523</v>
       </c>
       <c r="D49" s="98" t="n">
         <f aca="false">13-6</f>
@@ -24390,7 +24386,7 @@
       </c>
       <c r="E49" s="98"/>
       <c r="F49" s="136" t="s">
-        <v>1523</v>
+        <v>1524</v>
       </c>
       <c r="G49" s="102" t="n">
         <v>5</v>
@@ -24426,7 +24422,7 @@
         <v>129</v>
       </c>
       <c r="T49" s="167" t="s">
-        <v>1524</v>
+        <v>1525</v>
       </c>
       <c r="U49" s="167"/>
       <c r="V49" s="167"/>
@@ -24438,11 +24434,11 @@
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="209" t="s">
-        <v>1525</v>
+        <v>1526</v>
       </c>
       <c r="B50" s="203"/>
       <c r="C50" s="203" t="s">
-        <v>1526</v>
+        <v>1527</v>
       </c>
       <c r="D50" s="203" t="n">
         <f aca="false">13-6</f>
@@ -24450,7 +24446,7 @@
       </c>
       <c r="E50" s="203"/>
       <c r="F50" s="203" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="G50" s="209" t="n">
         <v>5</v>
@@ -24496,13 +24492,13 @@
     </row>
     <row r="51" customFormat="false" ht="25.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="102" t="s">
-        <v>1528</v>
+        <v>1529</v>
       </c>
       <c r="B51" s="98" t="s">
-        <v>1529</v>
+        <v>1530</v>
       </c>
       <c r="C51" s="98" t="s">
-        <v>1530</v>
+        <v>1531</v>
       </c>
       <c r="D51" s="98" t="n">
         <f aca="false">45-17</f>
@@ -24527,7 +24523,7 @@
       <c r="R51" s="102"/>
       <c r="S51" s="102"/>
       <c r="T51" s="167" t="s">
-        <v>1531</v>
+        <v>1532</v>
       </c>
       <c r="U51" s="167"/>
       <c r="V51" s="167"/>
@@ -24539,11 +24535,11 @@
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="209" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="B52" s="203"/>
       <c r="C52" s="203" t="s">
-        <v>1530</v>
+        <v>1531</v>
       </c>
       <c r="D52" s="203" t="n">
         <f aca="false">37-17</f>
@@ -24577,13 +24573,13 @@
     </row>
     <row r="53" customFormat="false" ht="25.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="102" t="s">
-        <v>1533</v>
+        <v>1534</v>
       </c>
       <c r="B53" s="136" t="s">
-        <v>1534</v>
+        <v>1535</v>
       </c>
       <c r="C53" s="98" t="s">
-        <v>1535</v>
+        <v>1536</v>
       </c>
       <c r="D53" s="98" t="s">
         <v>148</v>
@@ -24638,11 +24634,11 @@
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="209" t="s">
-        <v>1536</v>
+        <v>1537</v>
       </c>
       <c r="B54" s="203"/>
       <c r="C54" s="203" t="s">
-        <v>1535</v>
+        <v>1536</v>
       </c>
       <c r="D54" s="203"/>
       <c r="E54" s="203"/>
@@ -24680,24 +24676,24 @@
       <c r="S54" s="209" t="s">
         <v>129</v>
       </c>
-      <c r="T54" s="334"/>
-      <c r="U54" s="334"/>
-      <c r="V54" s="334"/>
-      <c r="W54" s="334"/>
-      <c r="X54" s="334"/>
-      <c r="Y54" s="334"/>
-      <c r="Z54" s="334"/>
-      <c r="AA54" s="334"/>
+      <c r="T54" s="333"/>
+      <c r="U54" s="333"/>
+      <c r="V54" s="333"/>
+      <c r="W54" s="333"/>
+      <c r="X54" s="333"/>
+      <c r="Y54" s="333"/>
+      <c r="Z54" s="333"/>
+      <c r="AA54" s="333"/>
     </row>
     <row r="55" customFormat="false" ht="49.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="102" t="s">
-        <v>1537</v>
+        <v>1538</v>
       </c>
       <c r="B55" s="136" t="s">
-        <v>1538</v>
+        <v>1539</v>
       </c>
       <c r="C55" s="136" t="s">
-        <v>1539</v>
+        <v>1540</v>
       </c>
       <c r="D55" s="102" t="n">
         <v>19</v>
@@ -24727,7 +24723,7 @@
       <c r="M55" s="102"/>
       <c r="N55" s="102"/>
       <c r="O55" s="173" t="s">
-        <v>1540</v>
+        <v>1541</v>
       </c>
       <c r="P55" s="102" t="n">
         <v>4</v>
@@ -24742,7 +24738,7 @@
         <v>275</v>
       </c>
       <c r="T55" s="167" t="s">
-        <v>1541</v>
+        <v>1542</v>
       </c>
       <c r="U55" s="167"/>
       <c r="V55" s="167"/>
@@ -24772,18 +24768,18 @@
       <c r="Q56" s="209"/>
       <c r="R56" s="209"/>
       <c r="S56" s="209"/>
-      <c r="T56" s="334"/>
-      <c r="U56" s="334"/>
-      <c r="V56" s="334"/>
-      <c r="W56" s="334"/>
-      <c r="X56" s="334"/>
-      <c r="Y56" s="334"/>
-      <c r="Z56" s="334"/>
-      <c r="AA56" s="334"/>
+      <c r="T56" s="333"/>
+      <c r="U56" s="333"/>
+      <c r="V56" s="333"/>
+      <c r="W56" s="333"/>
+      <c r="X56" s="333"/>
+      <c r="Y56" s="333"/>
+      <c r="Z56" s="333"/>
+      <c r="AA56" s="333"/>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="102" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="K57" s="136"/>
       <c r="L57" s="173"/>
@@ -24794,15 +24790,15 @@
       <c r="Q57" s="102"/>
       <c r="R57" s="102"/>
       <c r="S57" s="175"/>
-      <c r="T57" s="336" t="s">
-        <v>1543</v>
-      </c>
-      <c r="U57" s="336"/>
-      <c r="V57" s="336"/>
-      <c r="W57" s="336"/>
-      <c r="X57" s="336"/>
-      <c r="Y57" s="336"/>
-      <c r="Z57" s="336"/>
+      <c r="T57" s="335" t="s">
+        <v>1544</v>
+      </c>
+      <c r="U57" s="335"/>
+      <c r="V57" s="335"/>
+      <c r="W57" s="335"/>
+      <c r="X57" s="335"/>
+      <c r="Y57" s="335"/>
+      <c r="Z57" s="335"/>
     </row>
     <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -24892,7 +24888,7 @@
       <selection pane="bottomRight" activeCell="L35" activeCellId="0" sqref="L35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="40.14"/>
@@ -24909,8 +24905,8 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="337" t="s">
-        <v>1544</v>
+      <c r="A1" s="336" t="s">
+        <v>1545</v>
       </c>
       <c r="B1" s="159"/>
       <c r="C1" s="159"/>
@@ -24918,21 +24914,21 @@
       <c r="E1" s="159"/>
       <c r="F1" s="159"/>
       <c r="G1" s="159"/>
-      <c r="H1" s="338"/>
-      <c r="I1" s="338"/>
-      <c r="J1" s="338"/>
-      <c r="K1" s="338"/>
-      <c r="L1" s="338"/>
-      <c r="M1" s="338"/>
-      <c r="N1" s="338"/>
-      <c r="O1" s="338"/>
-      <c r="P1" s="338"/>
-      <c r="Q1" s="338"/>
-      <c r="R1" s="338"/>
-      <c r="S1" s="338"/>
-      <c r="T1" s="338"/>
-      <c r="U1" s="338"/>
-      <c r="V1" s="338"/>
+      <c r="H1" s="337"/>
+      <c r="I1" s="337"/>
+      <c r="J1" s="337"/>
+      <c r="K1" s="337"/>
+      <c r="L1" s="337"/>
+      <c r="M1" s="337"/>
+      <c r="N1" s="337"/>
+      <c r="O1" s="337"/>
+      <c r="P1" s="337"/>
+      <c r="Q1" s="337"/>
+      <c r="R1" s="337"/>
+      <c r="S1" s="337"/>
+      <c r="T1" s="337"/>
+      <c r="U1" s="337"/>
+      <c r="V1" s="337"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="160" t="s">
@@ -24977,7 +24973,7 @@
       <c r="N2" s="160" t="s">
         <v>119</v>
       </c>
-      <c r="O2" s="339" t="s">
+      <c r="O2" s="338" t="s">
         <v>55</v>
       </c>
       <c r="P2" s="88" t="s">
@@ -25002,62 +24998,62 @@
       <c r="Y2" s="217"/>
     </row>
     <row r="3" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="340" t="s">
+      <c r="A3" s="339" t="s">
         <v>122</v>
       </c>
-      <c r="B3" s="340" t="s">
+      <c r="B3" s="339" t="s">
         <v>299</v>
       </c>
-      <c r="C3" s="340" t="s">
+      <c r="C3" s="339" t="s">
         <v>578</v>
       </c>
-      <c r="D3" s="341" t="s">
+      <c r="D3" s="340" t="s">
         <v>950</v>
       </c>
-      <c r="F3" s="340" t="s">
+      <c r="F3" s="339" t="s">
         <v>155</v>
       </c>
-      <c r="G3" s="340" t="s">
+      <c r="G3" s="339" t="s">
         <v>297</v>
       </c>
-      <c r="H3" s="340" t="s">
+      <c r="H3" s="339" t="s">
         <v>298</v>
       </c>
-      <c r="I3" s="340" t="s">
+      <c r="I3" s="339" t="s">
         <v>299</v>
       </c>
-      <c r="J3" s="340" t="s">
+      <c r="J3" s="339" t="s">
         <v>127</v>
       </c>
-      <c r="K3" s="340" t="s">
+      <c r="K3" s="339" t="s">
         <v>312</v>
       </c>
-      <c r="L3" s="340" t="s">
+      <c r="L3" s="339" t="s">
         <v>128</v>
       </c>
-      <c r="M3" s="340"/>
-      <c r="N3" s="340"/>
-      <c r="O3" s="340"/>
-      <c r="P3" s="340" t="s">
+      <c r="M3" s="339"/>
+      <c r="N3" s="339"/>
+      <c r="O3" s="339"/>
+      <c r="P3" s="339" t="s">
         <v>299</v>
       </c>
-      <c r="Q3" s="340" t="s">
+      <c r="Q3" s="339" t="s">
         <v>127</v>
       </c>
-      <c r="R3" s="340" t="s">
+      <c r="R3" s="339" t="s">
         <v>138</v>
       </c>
-      <c r="S3" s="340" t="s">
-        <v>129</v>
-      </c>
-      <c r="T3" s="342" t="s">
+      <c r="S3" s="339" t="s">
+        <v>129</v>
+      </c>
+      <c r="T3" s="341" t="s">
         <v>419</v>
       </c>
-      <c r="U3" s="342"/>
-      <c r="V3" s="342"/>
-      <c r="W3" s="342"/>
-      <c r="X3" s="342"/>
-      <c r="Y3" s="342"/>
+      <c r="U3" s="341"/>
+      <c r="V3" s="341"/>
+      <c r="W3" s="341"/>
+      <c r="X3" s="341"/>
+      <c r="Y3" s="341"/>
     </row>
     <row r="4" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="97" t="s">
@@ -25073,7 +25069,7 @@
         <v>691</v>
       </c>
       <c r="F4" s="97" t="s">
-        <v>1545</v>
+        <v>1546</v>
       </c>
       <c r="G4" s="97" t="s">
         <v>168</v>
@@ -25116,61 +25112,61 @@
       <c r="Y4" s="101"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="340" t="s">
+      <c r="A5" s="339" t="s">
         <v>424</v>
       </c>
-      <c r="B5" s="340" t="s">
+      <c r="B5" s="339" t="s">
         <v>791</v>
       </c>
-      <c r="C5" s="340" t="s">
+      <c r="C5" s="339" t="s">
         <v>792</v>
       </c>
-      <c r="D5" s="340" t="n">
+      <c r="D5" s="339" t="n">
         <f aca="false">25-8</f>
         <v>17</v>
       </c>
-      <c r="F5" s="340" t="s">
-        <v>1546</v>
-      </c>
-      <c r="G5" s="340" t="s">
+      <c r="F5" s="339" t="s">
+        <v>1547</v>
+      </c>
+      <c r="G5" s="339" t="s">
         <v>138</v>
       </c>
-      <c r="H5" s="340" t="s">
+      <c r="H5" s="339" t="s">
         <v>444</v>
       </c>
-      <c r="I5" s="340" t="s">
+      <c r="I5" s="339" t="s">
         <v>161</v>
       </c>
-      <c r="J5" s="340" t="s">
+      <c r="J5" s="339" t="s">
         <v>235</v>
       </c>
-      <c r="K5" s="340" t="s">
+      <c r="K5" s="339" t="s">
         <v>297</v>
       </c>
-      <c r="L5" s="340" t="s">
+      <c r="L5" s="339" t="s">
         <v>128</v>
       </c>
-      <c r="M5" s="340"/>
-      <c r="N5" s="340"/>
-      <c r="O5" s="340"/>
-      <c r="P5" s="340" t="s">
+      <c r="M5" s="339"/>
+      <c r="N5" s="339"/>
+      <c r="O5" s="339"/>
+      <c r="P5" s="339" t="s">
         <v>159</v>
       </c>
-      <c r="Q5" s="340" t="s">
+      <c r="Q5" s="339" t="s">
         <v>183</v>
       </c>
-      <c r="R5" s="340" t="s">
+      <c r="R5" s="339" t="s">
         <v>138</v>
       </c>
-      <c r="S5" s="340" t="s">
-        <v>129</v>
-      </c>
-      <c r="T5" s="342"/>
-      <c r="U5" s="342"/>
-      <c r="V5" s="342"/>
-      <c r="W5" s="342"/>
-      <c r="X5" s="342"/>
-      <c r="Y5" s="342"/>
+      <c r="S5" s="339" t="s">
+        <v>129</v>
+      </c>
+      <c r="T5" s="341"/>
+      <c r="U5" s="341"/>
+      <c r="V5" s="341"/>
+      <c r="W5" s="341"/>
+      <c r="X5" s="341"/>
+      <c r="Y5" s="341"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="97" t="s">
@@ -25180,10 +25176,10 @@
         <v>138</v>
       </c>
       <c r="C6" s="97" t="s">
-        <v>1547</v>
+        <v>1548</v>
       </c>
       <c r="D6" s="97" t="s">
-        <v>1548</v>
+        <v>1549</v>
       </c>
       <c r="E6" s="97" t="n">
         <f aca="false">42-19</f>
@@ -25233,66 +25229,66 @@
       <c r="Y6" s="101"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="340" t="s">
-        <v>1549</v>
-      </c>
-      <c r="B7" s="340" t="s">
+      <c r="A7" s="339" t="s">
+        <v>1550</v>
+      </c>
+      <c r="B7" s="339" t="s">
         <v>138</v>
       </c>
-      <c r="C7" s="340" t="s">
-        <v>1547</v>
-      </c>
-      <c r="D7" s="340" t="s">
+      <c r="C7" s="339" t="s">
+        <v>1548</v>
+      </c>
+      <c r="D7" s="339" t="s">
         <v>297</v>
       </c>
-      <c r="E7" s="340" t="n">
+      <c r="E7" s="339" t="n">
         <f aca="false">27-19</f>
         <v>8</v>
       </c>
-      <c r="F7" s="340" t="s">
+      <c r="F7" s="339" t="s">
         <v>289</v>
       </c>
-      <c r="G7" s="340" t="s">
+      <c r="G7" s="339" t="s">
         <v>138</v>
       </c>
-      <c r="H7" s="340" t="s">
+      <c r="H7" s="339" t="s">
         <v>354</v>
       </c>
-      <c r="I7" s="340" t="s">
+      <c r="I7" s="339" t="s">
         <v>145</v>
       </c>
-      <c r="J7" s="340" t="s">
+      <c r="J7" s="339" t="s">
         <v>317</v>
       </c>
-      <c r="K7" s="340" t="s">
+      <c r="K7" s="339" t="s">
         <v>312</v>
       </c>
-      <c r="L7" s="340" t="s">
+      <c r="L7" s="339" t="s">
         <v>221</v>
       </c>
-      <c r="M7" s="340"/>
-      <c r="N7" s="340"/>
-      <c r="O7" s="340"/>
-      <c r="P7" s="340" t="s">
+      <c r="M7" s="339"/>
+      <c r="N7" s="339"/>
+      <c r="O7" s="339"/>
+      <c r="P7" s="339" t="s">
         <v>168</v>
       </c>
-      <c r="Q7" s="340" t="s">
+      <c r="Q7" s="339" t="s">
         <v>127</v>
       </c>
-      <c r="R7" s="340" t="s">
+      <c r="R7" s="339" t="s">
         <v>127</v>
       </c>
-      <c r="S7" s="340" t="s">
-        <v>129</v>
-      </c>
-      <c r="T7" s="343" t="s">
-        <v>1550</v>
-      </c>
-      <c r="U7" s="343"/>
-      <c r="V7" s="343"/>
-      <c r="W7" s="343"/>
-      <c r="X7" s="343"/>
-      <c r="Y7" s="343"/>
+      <c r="S7" s="339" t="s">
+        <v>129</v>
+      </c>
+      <c r="T7" s="342" t="s">
+        <v>1551</v>
+      </c>
+      <c r="U7" s="342"/>
+      <c r="V7" s="342"/>
+      <c r="W7" s="342"/>
+      <c r="X7" s="342"/>
+      <c r="Y7" s="342"/>
     </row>
     <row r="8" customFormat="false" ht="14.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="97" t="s">
@@ -25305,7 +25301,7 @@
         <v>699</v>
       </c>
       <c r="E8" s="109" t="s">
-        <v>1551</v>
+        <v>1552</v>
       </c>
       <c r="F8" s="97" t="s">
         <v>321</v>
@@ -25351,63 +25347,63 @@
       <c r="Y8" s="101"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="340" t="s">
+      <c r="A9" s="339" t="s">
         <v>441</v>
       </c>
-      <c r="B9" s="340"/>
-      <c r="C9" s="340" t="s">
-        <v>1552</v>
-      </c>
-      <c r="D9" s="340" t="s">
+      <c r="B9" s="339"/>
+      <c r="C9" s="339" t="s">
         <v>1553</v>
       </c>
-      <c r="E9" s="340"/>
-      <c r="F9" s="340"/>
-      <c r="G9" s="340" t="s">
+      <c r="D9" s="339" t="s">
+        <v>1554</v>
+      </c>
+      <c r="E9" s="339"/>
+      <c r="F9" s="339"/>
+      <c r="G9" s="339" t="s">
         <v>297</v>
       </c>
-      <c r="H9" s="340" t="s">
+      <c r="H9" s="339" t="s">
         <v>181</v>
       </c>
-      <c r="I9" s="340" t="s">
+      <c r="I9" s="339" t="s">
         <v>161</v>
       </c>
-      <c r="J9" s="340" t="s">
+      <c r="J9" s="339" t="s">
         <v>317</v>
       </c>
-      <c r="K9" s="340" t="s">
+      <c r="K9" s="339" t="s">
         <v>312</v>
       </c>
-      <c r="L9" s="340" t="s">
+      <c r="L9" s="339" t="s">
         <v>128</v>
       </c>
-      <c r="M9" s="340"/>
-      <c r="N9" s="340"/>
-      <c r="O9" s="340"/>
-      <c r="P9" s="340" t="s">
+      <c r="M9" s="339"/>
+      <c r="N9" s="339"/>
+      <c r="O9" s="339"/>
+      <c r="P9" s="339" t="s">
         <v>192</v>
       </c>
-      <c r="Q9" s="340" t="s">
+      <c r="Q9" s="339" t="s">
         <v>323</v>
       </c>
-      <c r="R9" s="340" t="s">
+      <c r="R9" s="339" t="s">
         <v>127</v>
       </c>
-      <c r="S9" s="340" t="s">
-        <v>129</v>
-      </c>
-      <c r="T9" s="342" t="s">
-        <v>1554</v>
-      </c>
-      <c r="U9" s="342"/>
-      <c r="V9" s="342"/>
-      <c r="W9" s="342"/>
-      <c r="X9" s="342"/>
-      <c r="Y9" s="342"/>
+      <c r="S9" s="339" t="s">
+        <v>129</v>
+      </c>
+      <c r="T9" s="341" t="s">
+        <v>1555</v>
+      </c>
+      <c r="U9" s="341"/>
+      <c r="V9" s="341"/>
+      <c r="W9" s="341"/>
+      <c r="X9" s="341"/>
+      <c r="Y9" s="341"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="97" t="s">
-        <v>1555</v>
+        <v>1556</v>
       </c>
       <c r="B10" s="97" t="s">
         <v>464</v>
@@ -25416,7 +25412,7 @@
         <v>1158</v>
       </c>
       <c r="D10" s="97" t="s">
-        <v>1556</v>
+        <v>1557</v>
       </c>
       <c r="E10" s="97" t="s">
         <v>147</v>
@@ -25458,7 +25454,7 @@
         <v>129</v>
       </c>
       <c r="T10" s="101" t="s">
-        <v>1557</v>
+        <v>1558</v>
       </c>
       <c r="U10" s="101"/>
       <c r="V10" s="101"/>
@@ -25467,59 +25463,59 @@
       <c r="Y10" s="101"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="340" t="s">
+      <c r="A11" s="339" t="s">
         <v>1156</v>
       </c>
-      <c r="B11" s="340"/>
-      <c r="C11" s="340" t="s">
+      <c r="B11" s="339"/>
+      <c r="C11" s="339" t="s">
         <v>1158</v>
       </c>
-      <c r="D11" s="340"/>
-      <c r="E11" s="340"/>
-      <c r="F11" s="340"/>
-      <c r="G11" s="340" t="s">
+      <c r="D11" s="339"/>
+      <c r="E11" s="339"/>
+      <c r="F11" s="339"/>
+      <c r="G11" s="339" t="s">
         <v>192</v>
       </c>
-      <c r="H11" s="340" t="s">
+      <c r="H11" s="339" t="s">
         <v>298</v>
       </c>
-      <c r="I11" s="340" t="s">
+      <c r="I11" s="339" t="s">
         <v>192</v>
       </c>
-      <c r="J11" s="340" t="s">
+      <c r="J11" s="339" t="s">
         <v>216</v>
       </c>
-      <c r="K11" s="340" t="s">
+      <c r="K11" s="339" t="s">
         <v>312</v>
       </c>
-      <c r="L11" s="340" t="s">
+      <c r="L11" s="339" t="s">
         <v>473</v>
       </c>
-      <c r="M11" s="340"/>
-      <c r="N11" s="340"/>
-      <c r="O11" s="340"/>
-      <c r="P11" s="340" t="s">
+      <c r="M11" s="339"/>
+      <c r="N11" s="339"/>
+      <c r="O11" s="339"/>
+      <c r="P11" s="339" t="s">
         <v>192</v>
       </c>
-      <c r="Q11" s="340" t="s">
+      <c r="Q11" s="339" t="s">
         <v>181</v>
       </c>
-      <c r="R11" s="340" t="s">
+      <c r="R11" s="339" t="s">
         <v>127</v>
       </c>
-      <c r="S11" s="340" t="s">
-        <v>129</v>
-      </c>
-      <c r="T11" s="342"/>
-      <c r="U11" s="342"/>
-      <c r="V11" s="342"/>
-      <c r="W11" s="342"/>
-      <c r="X11" s="342"/>
-      <c r="Y11" s="342"/>
+      <c r="S11" s="339" t="s">
+        <v>129</v>
+      </c>
+      <c r="T11" s="341"/>
+      <c r="U11" s="341"/>
+      <c r="V11" s="341"/>
+      <c r="W11" s="341"/>
+      <c r="X11" s="341"/>
+      <c r="Y11" s="341"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="97" t="s">
-        <v>1558</v>
+        <v>1559</v>
       </c>
       <c r="B12" s="97"/>
       <c r="C12" s="97" t="s">
@@ -25569,130 +25565,130 @@
       <c r="Y12" s="101"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="340" t="s">
+      <c r="A13" s="339" t="s">
         <v>167</v>
       </c>
-      <c r="B13" s="340" t="s">
+      <c r="B13" s="339" t="s">
         <v>138</v>
       </c>
-      <c r="C13" s="340" t="s">
+      <c r="C13" s="339" t="s">
         <v>139</v>
       </c>
-      <c r="D13" s="340" t="s">
-        <v>1559</v>
-      </c>
-      <c r="E13" s="340" t="s">
+      <c r="D13" s="339" t="s">
+        <v>1560</v>
+      </c>
+      <c r="E13" s="339" t="s">
         <v>304</v>
       </c>
-      <c r="F13" s="340" t="s">
+      <c r="F13" s="339" t="s">
         <v>366</v>
       </c>
-      <c r="G13" s="340" t="s">
+      <c r="G13" s="339" t="s">
         <v>145</v>
       </c>
-      <c r="H13" s="340" t="s">
+      <c r="H13" s="339" t="s">
         <v>327</v>
       </c>
-      <c r="I13" s="340" t="s">
+      <c r="I13" s="339" t="s">
         <v>138</v>
       </c>
-      <c r="J13" s="340" t="s">
+      <c r="J13" s="339" t="s">
         <v>317</v>
       </c>
-      <c r="K13" s="340" t="s">
+      <c r="K13" s="339" t="s">
         <v>314</v>
       </c>
-      <c r="L13" s="340" t="s">
+      <c r="L13" s="339" t="s">
         <v>128</v>
       </c>
-      <c r="M13" s="340"/>
-      <c r="N13" s="340"/>
-      <c r="O13" s="340"/>
-      <c r="P13" s="340" t="s">
+      <c r="M13" s="339"/>
+      <c r="N13" s="339"/>
+      <c r="O13" s="339"/>
+      <c r="P13" s="339" t="s">
         <v>145</v>
       </c>
-      <c r="Q13" s="340" t="s">
+      <c r="Q13" s="339" t="s">
         <v>155</v>
       </c>
-      <c r="R13" s="340" t="s">
+      <c r="R13" s="339" t="s">
         <v>138</v>
       </c>
-      <c r="S13" s="340" t="s">
-        <v>129</v>
-      </c>
-      <c r="T13" s="342" t="s">
-        <v>1560</v>
-      </c>
-      <c r="U13" s="342"/>
-      <c r="V13" s="342"/>
-      <c r="W13" s="342"/>
-      <c r="X13" s="342"/>
-      <c r="Y13" s="342"/>
+      <c r="S13" s="339" t="s">
+        <v>129</v>
+      </c>
+      <c r="T13" s="341" t="s">
+        <v>1561</v>
+      </c>
+      <c r="U13" s="341"/>
+      <c r="V13" s="341"/>
+      <c r="W13" s="341"/>
+      <c r="X13" s="341"/>
+      <c r="Y13" s="341"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="340" t="s">
+      <c r="A14" s="339" t="s">
         <v>814</v>
       </c>
-      <c r="B14" s="340" t="s">
+      <c r="B14" s="339" t="s">
         <v>299</v>
       </c>
-      <c r="C14" s="340" t="s">
+      <c r="C14" s="339" t="s">
         <v>892</v>
       </c>
-      <c r="D14" s="340" t="s">
+      <c r="D14" s="339" t="s">
         <v>159</v>
       </c>
-      <c r="E14" s="340" t="s">
+      <c r="E14" s="339" t="s">
         <v>183</v>
       </c>
-      <c r="F14" s="340" t="s">
+      <c r="F14" s="339" t="s">
         <v>140</v>
       </c>
-      <c r="G14" s="344" t="n">
+      <c r="G14" s="343" t="n">
         <v>4</v>
       </c>
-      <c r="H14" s="344" t="n">
+      <c r="H14" s="343" t="n">
         <v>30</v>
       </c>
-      <c r="I14" s="344" t="n">
+      <c r="I14" s="343" t="n">
         <v>7</v>
       </c>
-      <c r="J14" s="344" t="n">
+      <c r="J14" s="343" t="n">
         <v>20</v>
       </c>
-      <c r="K14" s="344" t="n">
+      <c r="K14" s="343" t="n">
         <v>2</v>
       </c>
-      <c r="L14" s="344" t="s">
+      <c r="L14" s="343" t="s">
         <v>251</v>
       </c>
-      <c r="M14" s="345" t="s">
+      <c r="M14" s="344" t="s">
         <v>299</v>
       </c>
       <c r="N14" s="163" t="s">
         <v>138</v>
       </c>
       <c r="O14" s="163"/>
-      <c r="P14" s="344" t="n">
+      <c r="P14" s="343" t="n">
         <v>6</v>
       </c>
-      <c r="Q14" s="340" t="s">
+      <c r="Q14" s="339" t="s">
         <v>323</v>
       </c>
-      <c r="R14" s="340" t="s">
+      <c r="R14" s="339" t="s">
         <v>138</v>
       </c>
-      <c r="S14" s="344" t="s">
-        <v>129</v>
-      </c>
-      <c r="T14" s="342"/>
-      <c r="U14" s="342"/>
-      <c r="V14" s="342"/>
-      <c r="W14" s="342"/>
+      <c r="S14" s="343" t="s">
+        <v>129</v>
+      </c>
+      <c r="T14" s="341"/>
+      <c r="U14" s="341"/>
+      <c r="V14" s="341"/>
+      <c r="W14" s="341"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="97" t="s">
-        <v>1561</v>
+        <v>1562</v>
       </c>
       <c r="B15" s="97"/>
       <c r="C15" s="97" t="s">
@@ -25741,7 +25737,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="97" t="s">
-        <v>1562</v>
+        <v>1563</v>
       </c>
       <c r="B16" s="97"/>
       <c r="C16" s="97" t="s">
@@ -25789,71 +25785,71 @@
       <c r="W16" s="101"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="340" t="s">
-        <v>1563</v>
-      </c>
-      <c r="B17" s="340" t="s">
+      <c r="A17" s="339" t="s">
+        <v>1564</v>
+      </c>
+      <c r="B17" s="339" t="s">
         <v>192</v>
       </c>
-      <c r="C17" s="340" t="s">
+      <c r="C17" s="339" t="s">
         <v>320</v>
       </c>
-      <c r="D17" s="340" t="n">
+      <c r="D17" s="339" t="n">
         <f aca="false">E17/3*2</f>
         <v>10</v>
       </c>
-      <c r="E17" s="340" t="n">
+      <c r="E17" s="339" t="n">
         <f aca="false">30-15</f>
         <v>15</v>
       </c>
-      <c r="F17" s="340" t="s">
+      <c r="F17" s="339" t="s">
         <v>148</v>
       </c>
-      <c r="G17" s="340" t="s">
+      <c r="G17" s="339" t="s">
         <v>145</v>
       </c>
-      <c r="H17" s="340" t="s">
+      <c r="H17" s="339" t="s">
         <v>235</v>
       </c>
-      <c r="I17" s="340" t="s">
+      <c r="I17" s="339" t="s">
         <v>145</v>
       </c>
-      <c r="J17" s="340" t="s">
+      <c r="J17" s="339" t="s">
         <v>235</v>
       </c>
-      <c r="K17" s="340" t="s">
+      <c r="K17" s="339" t="s">
         <v>138</v>
       </c>
-      <c r="L17" s="340" t="s">
+      <c r="L17" s="339" t="s">
         <v>221</v>
       </c>
-      <c r="M17" s="345" t="s">
+      <c r="M17" s="344" t="s">
         <v>299</v>
       </c>
       <c r="N17" s="163" t="s">
         <v>138</v>
       </c>
       <c r="O17" s="163"/>
-      <c r="P17" s="340" t="s">
+      <c r="P17" s="339" t="s">
         <v>138</v>
       </c>
-      <c r="Q17" s="340" t="s">
+      <c r="Q17" s="339" t="s">
         <v>183</v>
       </c>
-      <c r="R17" s="340" t="s">
+      <c r="R17" s="339" t="s">
         <v>138</v>
       </c>
-      <c r="S17" s="340" t="s">
-        <v>129</v>
-      </c>
-      <c r="T17" s="342"/>
-      <c r="U17" s="342"/>
-      <c r="V17" s="342"/>
-      <c r="W17" s="342"/>
+      <c r="S17" s="339" t="s">
+        <v>129</v>
+      </c>
+      <c r="T17" s="341"/>
+      <c r="U17" s="341"/>
+      <c r="V17" s="341"/>
+      <c r="W17" s="341"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="97" t="s">
-        <v>1564</v>
+        <v>1565</v>
       </c>
       <c r="B18" s="97"/>
       <c r="C18" s="97" t="s">
@@ -25901,53 +25897,53 @@
       <c r="W18" s="101"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="340" t="s">
-        <v>1565</v>
-      </c>
-      <c r="B19" s="340"/>
-      <c r="C19" s="340" t="s">
+      <c r="A19" s="339" t="s">
+        <v>1566</v>
+      </c>
+      <c r="B19" s="339"/>
+      <c r="C19" s="339" t="s">
         <v>326</v>
       </c>
-      <c r="D19" s="340"/>
-      <c r="E19" s="340"/>
-      <c r="F19" s="340"/>
-      <c r="G19" s="340" t="s">
+      <c r="D19" s="339"/>
+      <c r="E19" s="339"/>
+      <c r="F19" s="339"/>
+      <c r="G19" s="339" t="s">
         <v>168</v>
       </c>
-      <c r="H19" s="340" t="s">
+      <c r="H19" s="339" t="s">
         <v>298</v>
       </c>
-      <c r="I19" s="340" t="s">
+      <c r="I19" s="339" t="s">
         <v>168</v>
       </c>
-      <c r="J19" s="340" t="s">
+      <c r="J19" s="339" t="s">
         <v>317</v>
       </c>
-      <c r="K19" s="340" t="s">
+      <c r="K19" s="339" t="s">
         <v>314</v>
       </c>
-      <c r="L19" s="340" t="s">
+      <c r="L19" s="339" t="s">
         <v>221</v>
       </c>
-      <c r="M19" s="345"/>
+      <c r="M19" s="344"/>
       <c r="N19" s="163"/>
       <c r="O19" s="163"/>
-      <c r="P19" s="340" t="s">
+      <c r="P19" s="339" t="s">
         <v>168</v>
       </c>
-      <c r="Q19" s="340" t="s">
+      <c r="Q19" s="339" t="s">
         <v>317</v>
       </c>
-      <c r="R19" s="340" t="s">
+      <c r="R19" s="339" t="s">
         <v>138</v>
       </c>
-      <c r="S19" s="340" t="s">
-        <v>129</v>
-      </c>
-      <c r="T19" s="342"/>
-      <c r="U19" s="342"/>
-      <c r="V19" s="342"/>
-      <c r="W19" s="342"/>
+      <c r="S19" s="339" t="s">
+        <v>129</v>
+      </c>
+      <c r="T19" s="341"/>
+      <c r="U19" s="341"/>
+      <c r="V19" s="341"/>
+      <c r="W19" s="341"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="97" t="s">
@@ -26012,53 +26008,53 @@
       <c r="W20" s="101"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="340" t="s">
+      <c r="A21" s="339" t="s">
         <v>904</v>
       </c>
-      <c r="B21" s="340"/>
-      <c r="C21" s="340" t="s">
+      <c r="B21" s="339"/>
+      <c r="C21" s="339" t="s">
         <v>820</v>
       </c>
-      <c r="D21" s="340"/>
-      <c r="E21" s="340"/>
-      <c r="F21" s="340"/>
-      <c r="G21" s="340" t="s">
+      <c r="D21" s="339"/>
+      <c r="E21" s="339"/>
+      <c r="F21" s="339"/>
+      <c r="G21" s="339" t="s">
         <v>168</v>
       </c>
-      <c r="H21" s="340" t="s">
+      <c r="H21" s="339" t="s">
         <v>476</v>
       </c>
-      <c r="I21" s="340" t="s">
+      <c r="I21" s="339" t="s">
         <v>168</v>
       </c>
-      <c r="J21" s="340" t="s">
+      <c r="J21" s="339" t="s">
         <v>235</v>
       </c>
-      <c r="K21" s="340" t="s">
+      <c r="K21" s="339" t="s">
         <v>312</v>
       </c>
-      <c r="L21" s="340" t="s">
+      <c r="L21" s="339" t="s">
         <v>473</v>
       </c>
-      <c r="M21" s="345"/>
+      <c r="M21" s="344"/>
       <c r="N21" s="163"/>
       <c r="O21" s="163"/>
-      <c r="P21" s="340" t="s">
+      <c r="P21" s="339" t="s">
         <v>138</v>
       </c>
-      <c r="Q21" s="340" t="s">
+      <c r="Q21" s="339" t="s">
         <v>155</v>
       </c>
-      <c r="R21" s="340" t="s">
+      <c r="R21" s="339" t="s">
         <v>138</v>
       </c>
-      <c r="S21" s="340" t="s">
-        <v>129</v>
-      </c>
-      <c r="T21" s="342"/>
-      <c r="U21" s="342"/>
-      <c r="V21" s="342"/>
-      <c r="W21" s="342"/>
+      <c r="S21" s="339" t="s">
+        <v>129</v>
+      </c>
+      <c r="T21" s="341"/>
+      <c r="U21" s="341"/>
+      <c r="V21" s="341"/>
+      <c r="W21" s="341"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="97" t="s">
@@ -26124,53 +26120,53 @@
       <c r="W22" s="101"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="340" t="s">
+      <c r="A23" s="339" t="s">
         <v>642</v>
       </c>
-      <c r="B23" s="340"/>
-      <c r="C23" s="340" t="s">
-        <v>1566</v>
-      </c>
-      <c r="D23" s="340"/>
-      <c r="E23" s="340"/>
-      <c r="F23" s="340"/>
-      <c r="G23" s="340" t="s">
+      <c r="B23" s="339"/>
+      <c r="C23" s="339" t="s">
+        <v>1464</v>
+      </c>
+      <c r="D23" s="339"/>
+      <c r="E23" s="339"/>
+      <c r="F23" s="339"/>
+      <c r="G23" s="339" t="s">
         <v>168</v>
       </c>
-      <c r="H23" s="340" t="s">
+      <c r="H23" s="339" t="s">
         <v>327</v>
       </c>
-      <c r="I23" s="340" t="s">
+      <c r="I23" s="339" t="s">
         <v>138</v>
       </c>
-      <c r="J23" s="340" t="s">
+      <c r="J23" s="339" t="s">
         <v>141</v>
       </c>
-      <c r="K23" s="340" t="s">
+      <c r="K23" s="339" t="s">
         <v>314</v>
       </c>
-      <c r="L23" s="340" t="s">
+      <c r="L23" s="339" t="s">
         <v>217</v>
       </c>
-      <c r="M23" s="345"/>
+      <c r="M23" s="344"/>
       <c r="N23" s="163"/>
       <c r="O23" s="163"/>
-      <c r="P23" s="340" t="s">
+      <c r="P23" s="339" t="s">
         <v>138</v>
       </c>
-      <c r="Q23" s="340" t="s">
+      <c r="Q23" s="339" t="s">
         <v>159</v>
       </c>
-      <c r="R23" s="340" t="s">
+      <c r="R23" s="339" t="s">
         <v>138</v>
       </c>
-      <c r="S23" s="340" t="s">
-        <v>129</v>
-      </c>
-      <c r="T23" s="342"/>
-      <c r="U23" s="342"/>
-      <c r="V23" s="342"/>
-      <c r="W23" s="342"/>
+      <c r="S23" s="339" t="s">
+        <v>129</v>
+      </c>
+      <c r="T23" s="341"/>
+      <c r="U23" s="341"/>
+      <c r="V23" s="341"/>
+      <c r="W23" s="341"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="97" t="s">
@@ -26222,68 +26218,68 @@
       <c r="W24" s="101"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="340" t="s">
+      <c r="A25" s="339" t="s">
         <v>372</v>
       </c>
-      <c r="B25" s="340" t="s">
+      <c r="B25" s="339" t="s">
         <v>192</v>
       </c>
-      <c r="C25" s="340" t="s">
+      <c r="C25" s="339" t="s">
         <v>320</v>
       </c>
-      <c r="D25" s="340" t="s">
+      <c r="D25" s="339" t="s">
         <v>161</v>
       </c>
-      <c r="E25" s="340" t="n">
+      <c r="E25" s="339" t="n">
         <f aca="false">30-15</f>
         <v>15</v>
       </c>
-      <c r="F25" s="340" t="s">
+      <c r="F25" s="339" t="s">
         <v>148</v>
       </c>
-      <c r="G25" s="340" t="s">
+      <c r="G25" s="339" t="s">
         <v>145</v>
       </c>
-      <c r="H25" s="340" t="s">
+      <c r="H25" s="339" t="s">
         <v>298</v>
       </c>
-      <c r="I25" s="340" t="s">
+      <c r="I25" s="339" t="s">
         <v>145</v>
       </c>
-      <c r="J25" s="340" t="s">
+      <c r="J25" s="339" t="s">
         <v>317</v>
       </c>
-      <c r="K25" s="340" t="s">
+      <c r="K25" s="339" t="s">
         <v>314</v>
       </c>
-      <c r="L25" s="340" t="s">
+      <c r="L25" s="339" t="s">
         <v>468</v>
       </c>
-      <c r="M25" s="345" t="s">
+      <c r="M25" s="344" t="s">
         <v>138</v>
       </c>
       <c r="N25" s="163" t="s">
         <v>161</v>
       </c>
       <c r="O25" s="163"/>
-      <c r="P25" s="344" t="n">
+      <c r="P25" s="343" t="n">
         <v>8</v>
       </c>
-      <c r="Q25" s="340" t="s">
+      <c r="Q25" s="339" t="s">
         <v>141</v>
       </c>
-      <c r="R25" s="340" t="s">
+      <c r="R25" s="339" t="s">
         <v>299</v>
       </c>
-      <c r="S25" s="340" t="s">
-        <v>129</v>
-      </c>
-      <c r="T25" s="342" t="s">
+      <c r="S25" s="339" t="s">
+        <v>129</v>
+      </c>
+      <c r="T25" s="341" t="s">
         <v>707</v>
       </c>
-      <c r="U25" s="342"/>
-      <c r="V25" s="342"/>
-      <c r="W25" s="342"/>
+      <c r="U25" s="341"/>
+      <c r="V25" s="341"/>
+      <c r="W25" s="341"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="97" t="s">
@@ -26335,63 +26331,63 @@
       <c r="W26" s="101"/>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="340" t="s">
+      <c r="A27" s="339" t="s">
         <v>1157</v>
       </c>
-      <c r="B27" s="340" t="s">
+      <c r="B27" s="339" t="s">
         <v>214</v>
       </c>
-      <c r="C27" s="344" t="s">
+      <c r="C27" s="343" t="s">
         <v>731</v>
       </c>
-      <c r="D27" s="340" t="s">
+      <c r="D27" s="339" t="s">
         <v>1567</v>
       </c>
-      <c r="E27" s="340" t="s">
+      <c r="E27" s="339" t="s">
         <v>1568</v>
       </c>
-      <c r="F27" s="341" t="s">
+      <c r="F27" s="340" t="s">
         <v>1569</v>
       </c>
-      <c r="G27" s="344" t="n">
+      <c r="G27" s="343" t="n">
         <v>12</v>
       </c>
-      <c r="H27" s="344" t="n">
+      <c r="H27" s="343" t="n">
         <v>45</v>
       </c>
-      <c r="I27" s="340" t="s">
+      <c r="I27" s="339" t="s">
         <v>192</v>
       </c>
-      <c r="J27" s="340" t="s">
+      <c r="J27" s="339" t="s">
         <v>190</v>
       </c>
-      <c r="K27" s="340" t="s">
+      <c r="K27" s="339" t="s">
         <v>168</v>
       </c>
-      <c r="L27" s="340" t="s">
+      <c r="L27" s="339" t="s">
         <v>128</v>
       </c>
-      <c r="M27" s="340"/>
-      <c r="N27" s="340"/>
-      <c r="O27" s="340"/>
-      <c r="P27" s="340" t="s">
+      <c r="M27" s="339"/>
+      <c r="N27" s="339"/>
+      <c r="O27" s="339"/>
+      <c r="P27" s="339" t="s">
         <v>159</v>
       </c>
-      <c r="Q27" s="340" t="s">
+      <c r="Q27" s="339" t="s">
         <v>327</v>
       </c>
-      <c r="R27" s="340" t="s">
+      <c r="R27" s="339" t="s">
         <v>127</v>
       </c>
-      <c r="S27" s="340" t="s">
-        <v>129</v>
-      </c>
-      <c r="T27" s="343" t="s">
+      <c r="S27" s="339" t="s">
+        <v>129</v>
+      </c>
+      <c r="T27" s="342" t="s">
         <v>1570</v>
       </c>
-      <c r="U27" s="343"/>
-      <c r="V27" s="343"/>
-      <c r="W27" s="343"/>
+      <c r="U27" s="342"/>
+      <c r="V27" s="342"/>
+      <c r="W27" s="342"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="97" t="s">
@@ -26443,63 +26439,63 @@
       <c r="W28" s="101"/>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="340" t="s">
+      <c r="A29" s="339" t="s">
         <v>1162</v>
       </c>
-      <c r="B29" s="340" t="s">
+      <c r="B29" s="339" t="s">
         <v>229</v>
       </c>
-      <c r="C29" s="340" t="s">
+      <c r="C29" s="339" t="s">
         <v>638</v>
       </c>
-      <c r="D29" s="340" t="s">
+      <c r="D29" s="339" t="s">
         <v>1567</v>
       </c>
-      <c r="E29" s="340" t="s">
+      <c r="E29" s="339" t="s">
         <v>1568</v>
       </c>
-      <c r="F29" s="341" t="s">
+      <c r="F29" s="340" t="s">
         <v>1571</v>
       </c>
-      <c r="G29" s="340" t="s">
+      <c r="G29" s="339" t="s">
         <v>159</v>
       </c>
-      <c r="H29" s="340" t="s">
+      <c r="H29" s="339" t="s">
         <v>341</v>
       </c>
-      <c r="I29" s="344" t="n">
+      <c r="I29" s="343" t="n">
         <v>7</v>
       </c>
-      <c r="J29" s="340" t="s">
+      <c r="J29" s="339" t="s">
         <v>458</v>
       </c>
-      <c r="K29" s="340" t="s">
+      <c r="K29" s="339" t="s">
         <v>168</v>
       </c>
-      <c r="L29" s="340" t="s">
+      <c r="L29" s="339" t="s">
         <v>128</v>
       </c>
-      <c r="M29" s="340"/>
-      <c r="N29" s="340"/>
-      <c r="O29" s="340"/>
-      <c r="P29" s="340" t="s">
+      <c r="M29" s="339"/>
+      <c r="N29" s="339"/>
+      <c r="O29" s="339"/>
+      <c r="P29" s="339" t="s">
         <v>159</v>
       </c>
-      <c r="Q29" s="340" t="s">
+      <c r="Q29" s="339" t="s">
         <v>327</v>
       </c>
-      <c r="R29" s="340" t="s">
+      <c r="R29" s="339" t="s">
         <v>138</v>
       </c>
-      <c r="S29" s="340" t="s">
-        <v>129</v>
-      </c>
-      <c r="T29" s="343" t="s">
+      <c r="S29" s="339" t="s">
+        <v>129</v>
+      </c>
+      <c r="T29" s="342" t="s">
         <v>1572</v>
       </c>
-      <c r="U29" s="343"/>
-      <c r="V29" s="343"/>
-      <c r="W29" s="343"/>
+      <c r="U29" s="342"/>
+      <c r="V29" s="342"/>
+      <c r="W29" s="342"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="97" t="s">
@@ -26551,63 +26547,63 @@
       <c r="W30" s="101"/>
     </row>
     <row r="31" customFormat="false" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="340" t="s">
+      <c r="A31" s="339" t="s">
         <v>724</v>
       </c>
-      <c r="B31" s="340" t="s">
+      <c r="B31" s="339" t="s">
         <v>173</v>
       </c>
-      <c r="C31" s="340" t="s">
+      <c r="C31" s="339" t="s">
         <v>1574</v>
       </c>
-      <c r="D31" s="340" t="s">
+      <c r="D31" s="339" t="s">
         <v>173</v>
       </c>
-      <c r="E31" s="340" t="s">
+      <c r="E31" s="339" t="s">
         <v>1575</v>
       </c>
-      <c r="F31" s="341" t="s">
+      <c r="F31" s="340" t="s">
         <v>1576</v>
       </c>
-      <c r="G31" s="340" t="s">
+      <c r="G31" s="339" t="s">
         <v>192</v>
       </c>
-      <c r="H31" s="340" t="s">
+      <c r="H31" s="339" t="s">
         <v>541</v>
       </c>
-      <c r="I31" s="340" t="s">
+      <c r="I31" s="339" t="s">
         <v>138</v>
       </c>
-      <c r="J31" s="340" t="s">
+      <c r="J31" s="339" t="s">
         <v>235</v>
       </c>
-      <c r="K31" s="340" t="s">
+      <c r="K31" s="339" t="s">
         <v>314</v>
       </c>
-      <c r="L31" s="340" t="s">
+      <c r="L31" s="339" t="s">
         <v>128</v>
       </c>
-      <c r="M31" s="340"/>
-      <c r="N31" s="340"/>
-      <c r="O31" s="340"/>
-      <c r="P31" s="340" t="s">
+      <c r="M31" s="339"/>
+      <c r="N31" s="339"/>
+      <c r="O31" s="339"/>
+      <c r="P31" s="339" t="s">
         <v>145</v>
       </c>
-      <c r="Q31" s="340" t="s">
+      <c r="Q31" s="339" t="s">
         <v>141</v>
       </c>
-      <c r="R31" s="340" t="s">
+      <c r="R31" s="339" t="s">
         <v>138</v>
       </c>
-      <c r="S31" s="340" t="s">
-        <v>129</v>
-      </c>
-      <c r="T31" s="342" t="s">
+      <c r="S31" s="339" t="s">
+        <v>129</v>
+      </c>
+      <c r="T31" s="341" t="s">
         <v>1577</v>
       </c>
-      <c r="U31" s="342"/>
-      <c r="V31" s="342"/>
-      <c r="W31" s="342"/>
+      <c r="U31" s="341"/>
+      <c r="V31" s="341"/>
+      <c r="W31" s="341"/>
     </row>
     <row r="32" customFormat="false" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="97" t="s">
@@ -26662,110 +26658,110 @@
       <c r="Y32" s="101"/>
     </row>
     <row r="33" customFormat="false" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="340" t="s">
+      <c r="A33" s="339" t="s">
         <v>1581</v>
       </c>
-      <c r="B33" s="340"/>
+      <c r="B33" s="339"/>
       <c r="C33" s="178" t="s">
         <v>1582</v>
       </c>
-      <c r="D33" s="340"/>
-      <c r="E33" s="340"/>
-      <c r="F33" s="340"/>
-      <c r="G33" s="340" t="s">
+      <c r="D33" s="339"/>
+      <c r="E33" s="339"/>
+      <c r="F33" s="339"/>
+      <c r="G33" s="339" t="s">
         <v>314</v>
       </c>
-      <c r="H33" s="340" t="s">
+      <c r="H33" s="339" t="s">
         <v>458</v>
       </c>
-      <c r="I33" s="340" t="s">
+      <c r="I33" s="339" t="s">
         <v>138</v>
       </c>
-      <c r="J33" s="340" t="s">
+      <c r="J33" s="339" t="s">
         <v>159</v>
       </c>
-      <c r="K33" s="340" t="s">
+      <c r="K33" s="339" t="s">
         <v>314</v>
       </c>
-      <c r="L33" s="340" t="s">
+      <c r="L33" s="339" t="s">
         <v>1308</v>
       </c>
-      <c r="M33" s="340"/>
-      <c r="N33" s="340"/>
-      <c r="O33" s="340"/>
-      <c r="P33" s="340" t="s">
+      <c r="M33" s="339"/>
+      <c r="N33" s="339"/>
+      <c r="O33" s="339"/>
+      <c r="P33" s="339" t="s">
         <v>297</v>
       </c>
-      <c r="Q33" s="340" t="s">
+      <c r="Q33" s="339" t="s">
         <v>159</v>
       </c>
-      <c r="R33" s="340" t="s">
+      <c r="R33" s="339" t="s">
         <v>127</v>
       </c>
-      <c r="S33" s="340" t="s">
-        <v>129</v>
-      </c>
-      <c r="T33" s="342" t="s">
+      <c r="S33" s="339" t="s">
+        <v>129</v>
+      </c>
+      <c r="T33" s="341" t="s">
         <v>1580</v>
       </c>
-      <c r="U33" s="342"/>
-      <c r="V33" s="342"/>
-      <c r="W33" s="342"/>
-      <c r="X33" s="342"/>
-      <c r="Y33" s="342"/>
+      <c r="U33" s="341"/>
+      <c r="V33" s="341"/>
+      <c r="W33" s="341"/>
+      <c r="X33" s="341"/>
+      <c r="Y33" s="341"/>
     </row>
     <row r="34" customFormat="false" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="340" t="s">
+      <c r="A34" s="339" t="s">
         <v>1581</v>
       </c>
-      <c r="B34" s="340"/>
+      <c r="B34" s="339"/>
       <c r="C34" s="178" t="s">
         <v>1582</v>
       </c>
-      <c r="D34" s="340"/>
-      <c r="E34" s="340"/>
-      <c r="F34" s="340"/>
-      <c r="G34" s="340" t="s">
+      <c r="D34" s="339"/>
+      <c r="E34" s="339"/>
+      <c r="F34" s="339"/>
+      <c r="G34" s="339" t="s">
         <v>314</v>
       </c>
-      <c r="H34" s="340" t="s">
+      <c r="H34" s="339" t="s">
         <v>428</v>
       </c>
-      <c r="I34" s="340" t="s">
+      <c r="I34" s="339" t="s">
         <v>138</v>
       </c>
-      <c r="J34" s="340" t="s">
+      <c r="J34" s="339" t="s">
         <v>159</v>
       </c>
-      <c r="K34" s="340" t="s">
+      <c r="K34" s="339" t="s">
         <v>314</v>
       </c>
-      <c r="L34" s="340" t="s">
+      <c r="L34" s="339" t="s">
         <v>128</v>
       </c>
-      <c r="M34" s="340"/>
-      <c r="N34" s="340"/>
-      <c r="O34" s="340"/>
-      <c r="P34" s="340" t="s">
+      <c r="M34" s="339"/>
+      <c r="N34" s="339"/>
+      <c r="O34" s="339"/>
+      <c r="P34" s="339" t="s">
         <v>297</v>
       </c>
-      <c r="Q34" s="340" t="s">
+      <c r="Q34" s="339" t="s">
         <v>159</v>
       </c>
-      <c r="R34" s="340" t="s">
+      <c r="R34" s="339" t="s">
         <v>127</v>
       </c>
-      <c r="S34" s="340" t="s">
-        <v>129</v>
-      </c>
-      <c r="T34" s="342" t="s">
+      <c r="S34" s="339" t="s">
+        <v>129</v>
+      </c>
+      <c r="T34" s="341" t="s">
         <v>1580</v>
       </c>
-      <c r="U34" s="342"/>
-      <c r="V34" s="342"/>
-      <c r="W34" s="342"/>
-      <c r="X34" s="342"/>
-      <c r="Y34" s="342"/>
+      <c r="U34" s="341"/>
+      <c r="V34" s="341"/>
+      <c r="W34" s="341"/>
+      <c r="X34" s="341"/>
+      <c r="Y34" s="341"/>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="97" t="s">
@@ -26827,59 +26823,59 @@
       <c r="Y35" s="104"/>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="340" t="s">
+      <c r="A36" s="339" t="s">
         <v>1587</v>
       </c>
-      <c r="B36" s="340"/>
-      <c r="C36" s="341" t="s">
+      <c r="B36" s="339"/>
+      <c r="C36" s="340" t="s">
         <v>1584</v>
       </c>
-      <c r="D36" s="340"/>
-      <c r="E36" s="340"/>
-      <c r="F36" s="341" t="s">
+      <c r="D36" s="339"/>
+      <c r="E36" s="339"/>
+      <c r="F36" s="340" t="s">
         <v>1588</v>
       </c>
-      <c r="G36" s="340" t="s">
+      <c r="G36" s="339" t="s">
         <v>297</v>
       </c>
-      <c r="H36" s="340" t="s">
+      <c r="H36" s="339" t="s">
         <v>341</v>
       </c>
-      <c r="I36" s="340" t="s">
+      <c r="I36" s="339" t="s">
         <v>299</v>
       </c>
-      <c r="J36" s="340" t="s">
+      <c r="J36" s="339" t="s">
         <v>428</v>
       </c>
-      <c r="K36" s="340" t="s">
+      <c r="K36" s="339" t="s">
         <v>314</v>
       </c>
-      <c r="L36" s="340" t="s">
+      <c r="L36" s="339" t="s">
         <v>1589</v>
       </c>
-      <c r="M36" s="340"/>
-      <c r="N36" s="340"/>
-      <c r="O36" s="340"/>
-      <c r="P36" s="340" t="s">
+      <c r="M36" s="339"/>
+      <c r="N36" s="339"/>
+      <c r="O36" s="339"/>
+      <c r="P36" s="339" t="s">
         <v>297</v>
       </c>
-      <c r="Q36" s="340" t="s">
+      <c r="Q36" s="339" t="s">
         <v>148</v>
       </c>
-      <c r="R36" s="340" t="s">
+      <c r="R36" s="339" t="s">
         <v>127</v>
       </c>
-      <c r="S36" s="340" t="s">
-        <v>129</v>
-      </c>
-      <c r="T36" s="343" t="s">
+      <c r="S36" s="339" t="s">
+        <v>129</v>
+      </c>
+      <c r="T36" s="342" t="s">
         <v>1586</v>
       </c>
-      <c r="U36" s="343"/>
-      <c r="V36" s="343"/>
-      <c r="W36" s="343"/>
-      <c r="X36" s="343"/>
-      <c r="Y36" s="343"/>
+      <c r="U36" s="342"/>
+      <c r="V36" s="342"/>
+      <c r="W36" s="342"/>
+      <c r="X36" s="342"/>
+      <c r="Y36" s="342"/>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="97" t="s">
@@ -26943,64 +26939,64 @@
       <c r="Y37" s="104"/>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="340" t="s">
+      <c r="A38" s="339" t="s">
         <v>1594</v>
       </c>
-      <c r="B38" s="340" t="s">
+      <c r="B38" s="339" t="s">
         <v>299</v>
       </c>
-      <c r="C38" s="340" t="s">
+      <c r="C38" s="339" t="s">
         <v>168</v>
       </c>
-      <c r="D38" s="340" t="n">
+      <c r="D38" s="339" t="n">
         <f aca="false">33-14</f>
         <v>19</v>
       </c>
-      <c r="E38" s="340"/>
-      <c r="F38" s="341" t="s">
+      <c r="E38" s="339"/>
+      <c r="F38" s="340" t="s">
         <v>1595</v>
       </c>
-      <c r="G38" s="344" t="n">
+      <c r="G38" s="343" t="n">
         <v>10</v>
       </c>
-      <c r="H38" s="340" t="s">
+      <c r="H38" s="339" t="s">
         <v>171</v>
       </c>
-      <c r="I38" s="340" t="s">
+      <c r="I38" s="339" t="s">
         <v>161</v>
       </c>
-      <c r="J38" s="340" t="s">
+      <c r="J38" s="339" t="s">
         <v>476</v>
       </c>
-      <c r="K38" s="340" t="s">
+      <c r="K38" s="339" t="s">
         <v>314</v>
       </c>
-      <c r="L38" s="340" t="s">
+      <c r="L38" s="339" t="s">
         <v>128</v>
       </c>
-      <c r="M38" s="340"/>
-      <c r="N38" s="340"/>
-      <c r="O38" s="340"/>
-      <c r="P38" s="340" t="s">
+      <c r="M38" s="339"/>
+      <c r="N38" s="339"/>
+      <c r="O38" s="339"/>
+      <c r="P38" s="339" t="s">
         <v>159</v>
       </c>
-      <c r="Q38" s="340" t="s">
+      <c r="Q38" s="339" t="s">
         <v>327</v>
       </c>
-      <c r="R38" s="340" t="s">
+      <c r="R38" s="339" t="s">
         <v>127</v>
       </c>
-      <c r="S38" s="340" t="s">
+      <c r="S38" s="339" t="s">
         <v>275</v>
       </c>
-      <c r="T38" s="343" t="s">
+      <c r="T38" s="342" t="s">
         <v>1596</v>
       </c>
-      <c r="U38" s="343"/>
-      <c r="V38" s="343"/>
-      <c r="W38" s="343"/>
-      <c r="X38" s="343"/>
-      <c r="Y38" s="343"/>
+      <c r="U38" s="342"/>
+      <c r="V38" s="342"/>
+      <c r="W38" s="342"/>
+      <c r="X38" s="342"/>
+      <c r="Y38" s="342"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="97" t="s">
@@ -27054,55 +27050,55 @@
       <c r="Y39" s="101"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="340" t="s">
+      <c r="A40" s="339" t="s">
         <v>1598</v>
       </c>
-      <c r="B40" s="340"/>
-      <c r="C40" s="340" t="s">
+      <c r="B40" s="339"/>
+      <c r="C40" s="339" t="s">
         <v>728</v>
       </c>
-      <c r="D40" s="340"/>
-      <c r="E40" s="340"/>
-      <c r="F40" s="340"/>
-      <c r="G40" s="340" t="s">
+      <c r="D40" s="339"/>
+      <c r="E40" s="339"/>
+      <c r="F40" s="339"/>
+      <c r="G40" s="339" t="s">
         <v>145</v>
       </c>
-      <c r="H40" s="340" t="s">
+      <c r="H40" s="339" t="s">
         <v>341</v>
       </c>
-      <c r="I40" s="340" t="s">
+      <c r="I40" s="339" t="s">
         <v>138</v>
       </c>
-      <c r="J40" s="340" t="s">
+      <c r="J40" s="339" t="s">
         <v>317</v>
       </c>
-      <c r="K40" s="340" t="s">
+      <c r="K40" s="339" t="s">
         <v>314</v>
       </c>
-      <c r="L40" s="340" t="s">
+      <c r="L40" s="339" t="s">
         <v>128</v>
       </c>
-      <c r="M40" s="340"/>
-      <c r="N40" s="340"/>
-      <c r="O40" s="340"/>
-      <c r="P40" s="340" t="s">
+      <c r="M40" s="339"/>
+      <c r="N40" s="339"/>
+      <c r="O40" s="339"/>
+      <c r="P40" s="339" t="s">
         <v>168</v>
       </c>
-      <c r="Q40" s="340" t="s">
+      <c r="Q40" s="339" t="s">
         <v>127</v>
       </c>
-      <c r="R40" s="340" t="s">
+      <c r="R40" s="339" t="s">
         <v>138</v>
       </c>
-      <c r="S40" s="340" t="s">
+      <c r="S40" s="339" t="s">
         <v>275</v>
       </c>
-      <c r="T40" s="342"/>
-      <c r="U40" s="342"/>
-      <c r="V40" s="342"/>
-      <c r="W40" s="342"/>
-      <c r="X40" s="342"/>
-      <c r="Y40" s="342"/>
+      <c r="T40" s="341"/>
+      <c r="U40" s="341"/>
+      <c r="V40" s="341"/>
+      <c r="W40" s="341"/>
+      <c r="X40" s="341"/>
+      <c r="Y40" s="341"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="97" t="s">
@@ -27164,63 +27160,63 @@
       <c r="Y41" s="101"/>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="340" t="s">
+      <c r="A42" s="339" t="s">
         <v>1602</v>
       </c>
-      <c r="B42" s="340" t="s">
+      <c r="B42" s="339" t="s">
         <v>229</v>
       </c>
-      <c r="C42" s="340" t="s">
+      <c r="C42" s="339" t="s">
         <v>1599</v>
       </c>
-      <c r="D42" s="341" t="s">
+      <c r="D42" s="340" t="s">
         <v>1603</v>
       </c>
-      <c r="E42" s="341"/>
-      <c r="F42" s="341" t="s">
+      <c r="E42" s="340"/>
+      <c r="F42" s="340" t="s">
         <v>1588</v>
       </c>
-      <c r="G42" s="340" t="s">
+      <c r="G42" s="339" t="s">
         <v>299</v>
       </c>
-      <c r="H42" s="340" t="s">
+      <c r="H42" s="339" t="s">
         <v>171</v>
       </c>
-      <c r="I42" s="340" t="s">
+      <c r="I42" s="339" t="s">
         <v>138</v>
       </c>
-      <c r="J42" s="340" t="s">
+      <c r="J42" s="339" t="s">
         <v>323</v>
       </c>
-      <c r="K42" s="340" t="s">
+      <c r="K42" s="339" t="s">
         <v>314</v>
       </c>
-      <c r="L42" s="340" t="s">
+      <c r="L42" s="339" t="s">
         <v>128</v>
       </c>
-      <c r="M42" s="340"/>
-      <c r="N42" s="340"/>
-      <c r="O42" s="340"/>
-      <c r="P42" s="344" t="n">
+      <c r="M42" s="339"/>
+      <c r="N42" s="339"/>
+      <c r="O42" s="339"/>
+      <c r="P42" s="343" t="n">
         <v>6</v>
       </c>
-      <c r="Q42" s="344" t="n">
-        <v>0</v>
-      </c>
-      <c r="R42" s="344" t="n">
-        <v>0</v>
-      </c>
-      <c r="S42" s="340" t="s">
-        <v>129</v>
-      </c>
-      <c r="T42" s="343" t="s">
+      <c r="Q42" s="343" t="n">
+        <v>0</v>
+      </c>
+      <c r="R42" s="343" t="n">
+        <v>0</v>
+      </c>
+      <c r="S42" s="339" t="s">
+        <v>129</v>
+      </c>
+      <c r="T42" s="342" t="s">
         <v>1604</v>
       </c>
-      <c r="U42" s="343"/>
-      <c r="V42" s="343"/>
-      <c r="W42" s="343"/>
-      <c r="X42" s="343"/>
-      <c r="Y42" s="343"/>
+      <c r="U42" s="342"/>
+      <c r="V42" s="342"/>
+      <c r="W42" s="342"/>
+      <c r="X42" s="342"/>
+      <c r="Y42" s="342"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="97" t="s">
@@ -27344,10 +27340,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="F3" activeCellId="0" sqref="F3"/>
+      <selection pane="topRight" activeCell="H29" activeCellId="0" sqref="H29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.14"/>
@@ -27363,31 +27359,31 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="346" t="s">
+      <c r="A1" s="345" t="s">
         <v>1608</v>
       </c>
-      <c r="B1" s="347"/>
-      <c r="C1" s="348"/>
-      <c r="D1" s="347"/>
-      <c r="E1" s="347"/>
-      <c r="F1" s="347"/>
-      <c r="G1" s="347"/>
-      <c r="H1" s="347"/>
-      <c r="I1" s="347"/>
-      <c r="J1" s="347"/>
-      <c r="K1" s="347"/>
-      <c r="L1" s="347"/>
-      <c r="M1" s="347"/>
-      <c r="N1" s="347"/>
-      <c r="O1" s="347"/>
-      <c r="P1" s="347"/>
-      <c r="Q1" s="347"/>
-      <c r="R1" s="347"/>
-      <c r="S1" s="347"/>
-      <c r="T1" s="347"/>
-      <c r="U1" s="347"/>
-      <c r="V1" s="347"/>
-      <c r="W1" s="347"/>
+      <c r="B1" s="346"/>
+      <c r="C1" s="347"/>
+      <c r="D1" s="346"/>
+      <c r="E1" s="346"/>
+      <c r="F1" s="346"/>
+      <c r="G1" s="346"/>
+      <c r="H1" s="346"/>
+      <c r="I1" s="346"/>
+      <c r="J1" s="346"/>
+      <c r="K1" s="346"/>
+      <c r="L1" s="346"/>
+      <c r="M1" s="346"/>
+      <c r="N1" s="346"/>
+      <c r="O1" s="346"/>
+      <c r="P1" s="346"/>
+      <c r="Q1" s="346"/>
+      <c r="R1" s="346"/>
+      <c r="S1" s="346"/>
+      <c r="T1" s="346"/>
+      <c r="U1" s="346"/>
+      <c r="V1" s="346"/>
+      <c r="W1" s="346"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="279" t="s">
@@ -27396,7 +27392,7 @@
       <c r="B2" s="279" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="349" t="s">
+      <c r="C2" s="348" t="s">
         <v>14</v>
       </c>
       <c r="D2" s="279" t="s">
@@ -27458,63 +27454,63 @@
       <c r="Z2" s="279"/>
     </row>
     <row r="3" customFormat="false" ht="24.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="350" t="s">
+      <c r="A3" s="349" t="s">
         <v>122</v>
       </c>
-      <c r="B3" s="351" t="n">
+      <c r="B3" s="350" t="n">
         <v>5</v>
       </c>
-      <c r="C3" s="352" t="s">
+      <c r="C3" s="351" t="s">
         <v>296</v>
       </c>
-      <c r="D3" s="353" t="s">
+      <c r="D3" s="352" t="s">
         <v>784</v>
       </c>
-      <c r="F3" s="351" t="n">
+      <c r="F3" s="350" t="n">
         <v>22</v>
       </c>
-      <c r="G3" s="351" t="n">
+      <c r="G3" s="350" t="n">
         <v>4</v>
       </c>
-      <c r="H3" s="351" t="n">
+      <c r="H3" s="350" t="n">
         <v>361</v>
       </c>
-      <c r="I3" s="351" t="n">
+      <c r="I3" s="350" t="n">
         <v>4</v>
       </c>
-      <c r="J3" s="351" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" s="351" t="n">
+      <c r="J3" s="350" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" s="350" t="n">
         <v>2</v>
       </c>
-      <c r="L3" s="351" t="s">
+      <c r="L3" s="350" t="s">
         <v>128</v>
       </c>
-      <c r="M3" s="351"/>
-      <c r="N3" s="351"/>
-      <c r="O3" s="351"/>
-      <c r="P3" s="351" t="n">
+      <c r="M3" s="350"/>
+      <c r="N3" s="350"/>
+      <c r="O3" s="350"/>
+      <c r="P3" s="350" t="n">
         <v>4</v>
       </c>
-      <c r="Q3" s="351" t="n">
-        <v>0</v>
-      </c>
-      <c r="R3" s="351" t="n">
+      <c r="Q3" s="350" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" s="350" t="n">
         <v>6</v>
       </c>
-      <c r="S3" s="351" t="s">
-        <v>129</v>
-      </c>
-      <c r="T3" s="354" t="s">
+      <c r="S3" s="350" t="s">
+        <v>129</v>
+      </c>
+      <c r="T3" s="353" t="s">
         <v>419</v>
       </c>
-      <c r="U3" s="354"/>
-      <c r="V3" s="354"/>
-      <c r="W3" s="354"/>
-      <c r="X3" s="354"/>
-      <c r="Y3" s="354"/>
-      <c r="Z3" s="354"/>
+      <c r="U3" s="353"/>
+      <c r="V3" s="353"/>
+      <c r="W3" s="353"/>
+      <c r="X3" s="353"/>
+      <c r="Y3" s="353"/>
+      <c r="Z3" s="353"/>
     </row>
     <row r="4" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="315" t="s">
@@ -27574,62 +27570,62 @@
       <c r="Z4" s="290"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="350" t="s">
+      <c r="A5" s="349" t="s">
         <v>424</v>
       </c>
-      <c r="B5" s="351" t="s">
+      <c r="B5" s="350" t="s">
         <v>1609</v>
       </c>
-      <c r="C5" s="352" t="s">
+      <c r="C5" s="351" t="s">
         <v>1610</v>
       </c>
-      <c r="D5" s="351" t="n">
+      <c r="D5" s="350" t="n">
         <f aca="false">52-35</f>
         <v>17</v>
       </c>
-      <c r="F5" s="351" t="s">
+      <c r="F5" s="350" t="s">
         <v>1611</v>
       </c>
-      <c r="G5" s="351" t="n">
+      <c r="G5" s="350" t="n">
         <v>6</v>
       </c>
-      <c r="H5" s="351" t="n">
+      <c r="H5" s="350" t="n">
         <v>361</v>
       </c>
-      <c r="I5" s="351" t="n">
+      <c r="I5" s="350" t="n">
         <v>8</v>
       </c>
-      <c r="J5" s="351" t="n">
+      <c r="J5" s="350" t="n">
         <v>50</v>
       </c>
-      <c r="K5" s="351" t="n">
+      <c r="K5" s="350" t="n">
         <v>3</v>
       </c>
-      <c r="L5" s="351" t="s">
+      <c r="L5" s="350" t="s">
         <v>128</v>
       </c>
-      <c r="M5" s="351"/>
-      <c r="N5" s="351"/>
-      <c r="O5" s="351"/>
-      <c r="P5" s="351" t="n">
+      <c r="M5" s="350"/>
+      <c r="N5" s="350"/>
+      <c r="O5" s="350"/>
+      <c r="P5" s="350" t="n">
         <v>12</v>
       </c>
-      <c r="Q5" s="351" t="n">
+      <c r="Q5" s="350" t="n">
         <v>70</v>
       </c>
-      <c r="R5" s="351" t="n">
+      <c r="R5" s="350" t="n">
         <v>6</v>
       </c>
-      <c r="S5" s="351" t="s">
-        <v>129</v>
-      </c>
-      <c r="T5" s="354"/>
-      <c r="U5" s="354"/>
-      <c r="V5" s="354"/>
-      <c r="W5" s="354"/>
-      <c r="X5" s="354"/>
-      <c r="Y5" s="354"/>
-      <c r="Z5" s="354"/>
+      <c r="S5" s="350" t="s">
+        <v>129</v>
+      </c>
+      <c r="T5" s="353"/>
+      <c r="U5" s="353"/>
+      <c r="V5" s="353"/>
+      <c r="W5" s="353"/>
+      <c r="X5" s="353"/>
+      <c r="Y5" s="353"/>
+      <c r="Z5" s="353"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="315" t="s">
@@ -27692,56 +27688,56 @@
       <c r="Z6" s="290"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="350" t="s">
+      <c r="A7" s="349" t="s">
         <v>302</v>
       </c>
-      <c r="B7" s="351"/>
-      <c r="C7" s="355" t="s">
+      <c r="B7" s="350"/>
+      <c r="C7" s="354" t="s">
         <v>634</v>
       </c>
-      <c r="D7" s="351"/>
-      <c r="E7" s="351"/>
-      <c r="F7" s="351"/>
-      <c r="G7" s="351" t="n">
+      <c r="D7" s="350"/>
+      <c r="E7" s="350"/>
+      <c r="F7" s="350"/>
+      <c r="G7" s="350" t="n">
         <v>8</v>
       </c>
-      <c r="H7" s="351" t="n">
+      <c r="H7" s="350" t="n">
         <v>361</v>
       </c>
-      <c r="I7" s="351" t="n">
+      <c r="I7" s="350" t="n">
         <v>6</v>
       </c>
-      <c r="J7" s="351" t="n">
+      <c r="J7" s="350" t="n">
         <v>35</v>
       </c>
-      <c r="K7" s="351" t="n">
+      <c r="K7" s="350" t="n">
         <v>2</v>
       </c>
-      <c r="L7" s="351" t="s">
+      <c r="L7" s="350" t="s">
         <v>128</v>
       </c>
-      <c r="M7" s="351"/>
-      <c r="N7" s="351"/>
-      <c r="O7" s="351"/>
-      <c r="P7" s="351" t="n">
+      <c r="M7" s="350"/>
+      <c r="N7" s="350"/>
+      <c r="O7" s="350"/>
+      <c r="P7" s="350" t="n">
         <v>5</v>
       </c>
-      <c r="Q7" s="351" t="n">
+      <c r="Q7" s="350" t="n">
         <v>25</v>
       </c>
-      <c r="R7" s="351" t="n">
+      <c r="R7" s="350" t="n">
         <v>6</v>
       </c>
-      <c r="S7" s="351" t="s">
-        <v>129</v>
-      </c>
-      <c r="T7" s="354"/>
-      <c r="U7" s="354"/>
-      <c r="V7" s="354"/>
-      <c r="W7" s="354"/>
-      <c r="X7" s="354"/>
-      <c r="Y7" s="354"/>
-      <c r="Z7" s="354"/>
+      <c r="S7" s="350" t="s">
+        <v>129</v>
+      </c>
+      <c r="T7" s="353"/>
+      <c r="U7" s="353"/>
+      <c r="V7" s="353"/>
+      <c r="W7" s="353"/>
+      <c r="X7" s="353"/>
+      <c r="Y7" s="353"/>
+      <c r="Z7" s="353"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="315" t="s">
@@ -27807,56 +27803,56 @@
       <c r="Z8" s="290"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="350" t="s">
+      <c r="A9" s="349" t="s">
         <v>1150</v>
       </c>
-      <c r="B9" s="351"/>
-      <c r="C9" s="352" t="s">
-        <v>1566</v>
-      </c>
-      <c r="D9" s="351"/>
-      <c r="E9" s="351"/>
-      <c r="F9" s="351"/>
-      <c r="G9" s="351" t="n">
+      <c r="B9" s="350"/>
+      <c r="C9" s="351" t="s">
+        <v>1464</v>
+      </c>
+      <c r="D9" s="350"/>
+      <c r="E9" s="350"/>
+      <c r="F9" s="350"/>
+      <c r="G9" s="350" t="n">
         <v>5</v>
       </c>
-      <c r="H9" s="351" t="n">
+      <c r="H9" s="350" t="n">
         <v>361</v>
       </c>
-      <c r="I9" s="351" t="n">
+      <c r="I9" s="350" t="n">
         <v>7</v>
       </c>
-      <c r="J9" s="351" t="n">
+      <c r="J9" s="350" t="n">
         <v>65</v>
       </c>
-      <c r="K9" s="351" t="n">
+      <c r="K9" s="350" t="n">
         <v>1</v>
       </c>
-      <c r="L9" s="351" t="s">
+      <c r="L9" s="350" t="s">
         <v>128</v>
       </c>
-      <c r="M9" s="351"/>
-      <c r="N9" s="351"/>
-      <c r="O9" s="351"/>
-      <c r="P9" s="351" t="n">
+      <c r="M9" s="350"/>
+      <c r="N9" s="350"/>
+      <c r="O9" s="350"/>
+      <c r="P9" s="350" t="n">
         <v>6</v>
       </c>
-      <c r="Q9" s="351" t="n">
+      <c r="Q9" s="350" t="n">
         <v>50</v>
       </c>
-      <c r="R9" s="351" t="n">
+      <c r="R9" s="350" t="n">
         <v>6</v>
       </c>
-      <c r="S9" s="351" t="s">
-        <v>129</v>
-      </c>
-      <c r="T9" s="354"/>
-      <c r="U9" s="354"/>
-      <c r="V9" s="354"/>
-      <c r="W9" s="354"/>
-      <c r="X9" s="354"/>
-      <c r="Y9" s="354"/>
-      <c r="Z9" s="354"/>
+      <c r="S9" s="350" t="s">
+        <v>129</v>
+      </c>
+      <c r="T9" s="353"/>
+      <c r="U9" s="353"/>
+      <c r="V9" s="353"/>
+      <c r="W9" s="353"/>
+      <c r="X9" s="353"/>
+      <c r="Y9" s="353"/>
+      <c r="Z9" s="353"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="315" t="s">
@@ -27921,56 +27917,56 @@
       <c r="Z10" s="290"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="350" t="s">
+      <c r="A11" s="349" t="s">
         <v>325</v>
       </c>
-      <c r="B11" s="351"/>
-      <c r="C11" s="352" t="s">
-        <v>1566</v>
-      </c>
-      <c r="D11" s="351"/>
-      <c r="E11" s="351"/>
-      <c r="F11" s="351"/>
-      <c r="G11" s="351" t="n">
+      <c r="B11" s="350"/>
+      <c r="C11" s="351" t="s">
+        <v>1464</v>
+      </c>
+      <c r="D11" s="350"/>
+      <c r="E11" s="350"/>
+      <c r="F11" s="350"/>
+      <c r="G11" s="350" t="n">
         <v>8</v>
       </c>
-      <c r="H11" s="351" t="n">
+      <c r="H11" s="350" t="n">
         <v>90</v>
       </c>
-      <c r="I11" s="351" t="n">
+      <c r="I11" s="350" t="n">
         <v>8</v>
       </c>
-      <c r="J11" s="351" t="n">
+      <c r="J11" s="350" t="n">
         <v>20</v>
       </c>
-      <c r="K11" s="351" t="n">
+      <c r="K11" s="350" t="n">
         <v>1</v>
       </c>
-      <c r="L11" s="351" t="s">
+      <c r="L11" s="350" t="s">
         <v>128</v>
       </c>
-      <c r="M11" s="351"/>
-      <c r="N11" s="351"/>
-      <c r="O11" s="351"/>
-      <c r="P11" s="351" t="n">
+      <c r="M11" s="350"/>
+      <c r="N11" s="350"/>
+      <c r="O11" s="350"/>
+      <c r="P11" s="350" t="n">
         <v>7</v>
       </c>
-      <c r="Q11" s="351" t="n">
+      <c r="Q11" s="350" t="n">
         <v>25</v>
       </c>
-      <c r="R11" s="351" t="n">
+      <c r="R11" s="350" t="n">
         <v>6</v>
       </c>
-      <c r="S11" s="351" t="s">
-        <v>129</v>
-      </c>
-      <c r="T11" s="354"/>
-      <c r="U11" s="354"/>
-      <c r="V11" s="354"/>
-      <c r="W11" s="354"/>
-      <c r="X11" s="354"/>
-      <c r="Y11" s="354"/>
-      <c r="Z11" s="354"/>
+      <c r="S11" s="350" t="s">
+        <v>129</v>
+      </c>
+      <c r="T11" s="353"/>
+      <c r="U11" s="353"/>
+      <c r="V11" s="353"/>
+      <c r="W11" s="353"/>
+      <c r="X11" s="353"/>
+      <c r="Y11" s="353"/>
+      <c r="Z11" s="353"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="315" t="s">
@@ -28025,66 +28021,66 @@
       <c r="Z12" s="290"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="350" t="s">
+      <c r="A13" s="349" t="s">
         <v>167</v>
       </c>
-      <c r="B13" s="351" t="n">
+      <c r="B13" s="350" t="n">
         <v>4</v>
       </c>
-      <c r="C13" s="352" t="s">
+      <c r="C13" s="351" t="s">
         <v>892</v>
       </c>
-      <c r="D13" s="351" t="n">
+      <c r="D13" s="350" t="n">
         <f aca="false">E13/3*2</f>
         <v>12</v>
       </c>
-      <c r="E13" s="351" t="n">
+      <c r="E13" s="350" t="n">
         <f aca="false">26-8</f>
         <v>18</v>
       </c>
-      <c r="F13" s="351" t="n">
+      <c r="F13" s="350" t="n">
         <v>26</v>
       </c>
-      <c r="G13" s="351" t="n">
+      <c r="G13" s="350" t="n">
         <v>9</v>
       </c>
-      <c r="H13" s="351" t="n">
+      <c r="H13" s="350" t="n">
         <v>361</v>
       </c>
-      <c r="I13" s="351" t="n">
+      <c r="I13" s="350" t="n">
         <v>6</v>
       </c>
-      <c r="J13" s="351" t="n">
+      <c r="J13" s="350" t="n">
         <v>30</v>
       </c>
-      <c r="K13" s="351" t="n">
+      <c r="K13" s="350" t="n">
         <v>1</v>
       </c>
-      <c r="L13" s="351" t="s">
+      <c r="L13" s="350" t="s">
         <v>128</v>
       </c>
-      <c r="M13" s="351"/>
-      <c r="N13" s="351"/>
-      <c r="O13" s="351"/>
-      <c r="P13" s="351" t="n">
+      <c r="M13" s="350"/>
+      <c r="N13" s="350"/>
+      <c r="O13" s="350"/>
+      <c r="P13" s="350" t="n">
         <v>7</v>
       </c>
-      <c r="Q13" s="351" t="n">
+      <c r="Q13" s="350" t="n">
         <v>25</v>
       </c>
-      <c r="R13" s="351" t="n">
+      <c r="R13" s="350" t="n">
         <v>6</v>
       </c>
-      <c r="S13" s="351" t="s">
-        <v>129</v>
-      </c>
-      <c r="T13" s="354"/>
-      <c r="U13" s="354"/>
-      <c r="V13" s="354"/>
-      <c r="W13" s="354"/>
-      <c r="X13" s="354"/>
-      <c r="Y13" s="354"/>
-      <c r="Z13" s="354"/>
+      <c r="S13" s="350" t="s">
+        <v>129</v>
+      </c>
+      <c r="T13" s="353"/>
+      <c r="U13" s="353"/>
+      <c r="V13" s="353"/>
+      <c r="W13" s="353"/>
+      <c r="X13" s="353"/>
+      <c r="Y13" s="353"/>
+      <c r="Z13" s="353"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="315" t="s">
@@ -28150,56 +28146,56 @@
       <c r="Z14" s="290"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="350" t="s">
+      <c r="A15" s="349" t="s">
         <v>456</v>
       </c>
-      <c r="B15" s="351"/>
-      <c r="C15" s="352" t="s">
+      <c r="B15" s="350"/>
+      <c r="C15" s="351" t="s">
         <v>1616</v>
       </c>
-      <c r="D15" s="351"/>
-      <c r="E15" s="351"/>
-      <c r="F15" s="351"/>
-      <c r="G15" s="351" t="n">
+      <c r="D15" s="350"/>
+      <c r="E15" s="350"/>
+      <c r="F15" s="350"/>
+      <c r="G15" s="350" t="n">
         <v>8</v>
       </c>
-      <c r="H15" s="351" t="n">
+      <c r="H15" s="350" t="n">
         <v>361</v>
       </c>
-      <c r="I15" s="351" t="n">
+      <c r="I15" s="350" t="n">
         <v>8</v>
       </c>
-      <c r="J15" s="351" t="n">
+      <c r="J15" s="350" t="n">
         <v>90</v>
       </c>
-      <c r="K15" s="351" t="n">
+      <c r="K15" s="350" t="n">
         <v>1</v>
       </c>
-      <c r="L15" s="351" t="s">
+      <c r="L15" s="350" t="s">
         <v>128</v>
       </c>
-      <c r="M15" s="351"/>
-      <c r="N15" s="351"/>
-      <c r="O15" s="351"/>
-      <c r="P15" s="351" t="n">
+      <c r="M15" s="350"/>
+      <c r="N15" s="350"/>
+      <c r="O15" s="350"/>
+      <c r="P15" s="350" t="n">
         <v>8</v>
       </c>
-      <c r="Q15" s="351" t="n">
+      <c r="Q15" s="350" t="n">
         <v>50</v>
       </c>
-      <c r="R15" s="351" t="n">
-        <v>0</v>
-      </c>
-      <c r="S15" s="351" t="s">
-        <v>129</v>
-      </c>
-      <c r="T15" s="354"/>
-      <c r="U15" s="354"/>
-      <c r="V15" s="354"/>
-      <c r="W15" s="354"/>
-      <c r="X15" s="354"/>
-      <c r="Y15" s="354"/>
-      <c r="Z15" s="354"/>
+      <c r="R15" s="350" t="n">
+        <v>0</v>
+      </c>
+      <c r="S15" s="350" t="s">
+        <v>129</v>
+      </c>
+      <c r="T15" s="353"/>
+      <c r="U15" s="353"/>
+      <c r="V15" s="353"/>
+      <c r="W15" s="353"/>
+      <c r="X15" s="353"/>
+      <c r="Y15" s="353"/>
+      <c r="Z15" s="353"/>
     </row>
     <row r="16" customFormat="false" ht="24.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="315" t="s">
@@ -28258,66 +28254,66 @@
       <c r="Z16" s="290"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="350" t="s">
+      <c r="A17" s="349" t="s">
         <v>1620</v>
       </c>
-      <c r="B17" s="351" t="n">
+      <c r="B17" s="350" t="n">
         <v>11</v>
       </c>
-      <c r="C17" s="352" t="n">
+      <c r="C17" s="351" t="n">
         <v>12</v>
       </c>
-      <c r="D17" s="351" t="n">
+      <c r="D17" s="350" t="n">
         <f aca="false">E17/3*2</f>
         <v>24</v>
       </c>
-      <c r="E17" s="351" t="n">
+      <c r="E17" s="350" t="n">
         <f aca="false">49-13</f>
         <v>36</v>
       </c>
-      <c r="F17" s="351" t="n">
+      <c r="F17" s="350" t="n">
         <v>49</v>
       </c>
-      <c r="G17" s="351" t="n">
+      <c r="G17" s="350" t="n">
         <v>7</v>
       </c>
-      <c r="H17" s="351" t="n">
+      <c r="H17" s="350" t="n">
         <v>90</v>
       </c>
-      <c r="I17" s="351" t="n">
+      <c r="I17" s="350" t="n">
         <v>8</v>
       </c>
-      <c r="J17" s="351" t="n">
+      <c r="J17" s="350" t="n">
         <v>110</v>
       </c>
-      <c r="K17" s="351" t="n">
+      <c r="K17" s="350" t="n">
         <v>2</v>
       </c>
-      <c r="L17" s="351" t="s">
+      <c r="L17" s="350" t="s">
         <v>128</v>
       </c>
-      <c r="M17" s="351"/>
-      <c r="N17" s="351"/>
-      <c r="O17" s="351"/>
-      <c r="P17" s="351" t="n">
+      <c r="M17" s="350"/>
+      <c r="N17" s="350"/>
+      <c r="O17" s="350"/>
+      <c r="P17" s="350" t="n">
         <v>8</v>
       </c>
-      <c r="Q17" s="351" t="n">
+      <c r="Q17" s="350" t="n">
         <v>50</v>
       </c>
-      <c r="R17" s="351" t="n">
-        <v>0</v>
-      </c>
-      <c r="S17" s="351" t="s">
-        <v>129</v>
-      </c>
-      <c r="T17" s="354"/>
-      <c r="U17" s="354"/>
-      <c r="V17" s="354"/>
-      <c r="W17" s="354"/>
-      <c r="X17" s="354"/>
-      <c r="Y17" s="354"/>
-      <c r="Z17" s="354"/>
+      <c r="R17" s="350" t="n">
+        <v>0</v>
+      </c>
+      <c r="S17" s="350" t="s">
+        <v>129</v>
+      </c>
+      <c r="T17" s="353"/>
+      <c r="U17" s="353"/>
+      <c r="V17" s="353"/>
+      <c r="W17" s="353"/>
+      <c r="X17" s="353"/>
+      <c r="Y17" s="353"/>
+      <c r="Z17" s="353"/>
     </row>
     <row r="18" customFormat="false" ht="24.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="315" t="s">
@@ -28376,67 +28372,67 @@
       <c r="Z18" s="290"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="350" t="s">
+      <c r="A19" s="349" t="s">
         <v>191</v>
       </c>
-      <c r="B19" s="351" t="n">
+      <c r="B19" s="350" t="n">
         <v>4</v>
       </c>
-      <c r="C19" s="352" t="s">
+      <c r="C19" s="351" t="s">
         <v>1623</v>
       </c>
-      <c r="D19" s="351" t="n">
+      <c r="D19" s="350" t="n">
         <v>20</v>
       </c>
-      <c r="E19" s="351" t="n">
+      <c r="E19" s="350" t="n">
         <f aca="false">44-14</f>
         <v>30</v>
       </c>
-      <c r="F19" s="351" t="n">
+      <c r="F19" s="350" t="n">
         <v>44</v>
       </c>
-      <c r="G19" s="351" t="n">
+      <c r="G19" s="350" t="n">
         <v>5</v>
       </c>
-      <c r="H19" s="351" t="n">
-        <v>0</v>
-      </c>
-      <c r="I19" s="351" t="n">
+      <c r="H19" s="350" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" s="350" t="n">
         <v>8</v>
       </c>
-      <c r="J19" s="351" t="n">
-        <v>0</v>
-      </c>
-      <c r="K19" s="351" t="n">
+      <c r="J19" s="350" t="n">
+        <v>0</v>
+      </c>
+      <c r="K19" s="350" t="n">
         <v>2</v>
       </c>
-      <c r="L19" s="351" t="s">
+      <c r="L19" s="350" t="s">
         <v>857</v>
       </c>
-      <c r="M19" s="351"/>
-      <c r="N19" s="351"/>
-      <c r="O19" s="351"/>
-      <c r="P19" s="351" t="n">
+      <c r="M19" s="350"/>
+      <c r="N19" s="350"/>
+      <c r="O19" s="350"/>
+      <c r="P19" s="350" t="n">
         <v>7</v>
       </c>
-      <c r="Q19" s="351" t="n">
-        <v>0</v>
-      </c>
-      <c r="R19" s="351" t="n">
-        <v>0</v>
-      </c>
-      <c r="S19" s="351" t="s">
-        <v>129</v>
-      </c>
-      <c r="T19" s="354" t="s">
+      <c r="Q19" s="350" t="n">
+        <v>0</v>
+      </c>
+      <c r="R19" s="350" t="n">
+        <v>0</v>
+      </c>
+      <c r="S19" s="350" t="s">
+        <v>129</v>
+      </c>
+      <c r="T19" s="353" t="s">
         <v>1624</v>
       </c>
-      <c r="U19" s="354"/>
-      <c r="V19" s="354"/>
-      <c r="W19" s="354"/>
-      <c r="X19" s="354"/>
-      <c r="Y19" s="354"/>
-      <c r="Z19" s="354"/>
+      <c r="U19" s="353"/>
+      <c r="V19" s="353"/>
+      <c r="W19" s="353"/>
+      <c r="X19" s="353"/>
+      <c r="Y19" s="353"/>
+      <c r="Z19" s="353"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="315" t="s">
@@ -28491,65 +28487,65 @@
       <c r="Z20" s="290"/>
     </row>
     <row r="21" customFormat="false" ht="24.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="350" t="s">
+      <c r="A21" s="349" t="s">
         <v>1625</v>
       </c>
-      <c r="B21" s="351"/>
-      <c r="C21" s="352" t="s">
+      <c r="B21" s="350"/>
+      <c r="C21" s="351" t="s">
         <v>1161</v>
       </c>
-      <c r="D21" s="351" t="n">
+      <c r="D21" s="350" t="n">
         <v>19</v>
       </c>
-      <c r="E21" s="351"/>
-      <c r="F21" s="351"/>
-      <c r="G21" s="351" t="n">
+      <c r="E21" s="350"/>
+      <c r="F21" s="350"/>
+      <c r="G21" s="350" t="n">
         <v>10</v>
       </c>
-      <c r="H21" s="351" t="n">
+      <c r="H21" s="350" t="n">
         <v>45</v>
       </c>
-      <c r="I21" s="351" t="n">
+      <c r="I21" s="350" t="n">
         <v>8</v>
       </c>
-      <c r="J21" s="351" t="n">
+      <c r="J21" s="350" t="n">
         <v>115</v>
       </c>
-      <c r="K21" s="351" t="n">
+      <c r="K21" s="350" t="n">
         <v>3</v>
       </c>
-      <c r="L21" s="351" t="s">
+      <c r="L21" s="350" t="s">
         <v>128</v>
       </c>
-      <c r="M21" s="351"/>
-      <c r="N21" s="351"/>
-      <c r="O21" s="351"/>
-      <c r="P21" s="351" t="n">
+      <c r="M21" s="350"/>
+      <c r="N21" s="350"/>
+      <c r="O21" s="350"/>
+      <c r="P21" s="350" t="n">
         <v>18</v>
       </c>
-      <c r="Q21" s="351" t="n">
+      <c r="Q21" s="350" t="n">
         <v>50</v>
       </c>
-      <c r="R21" s="351" t="n">
-        <v>0</v>
-      </c>
-      <c r="S21" s="351" t="s">
-        <v>129</v>
-      </c>
-      <c r="T21" s="354" t="s">
+      <c r="R21" s="350" t="n">
+        <v>0</v>
+      </c>
+      <c r="S21" s="350" t="s">
+        <v>129</v>
+      </c>
+      <c r="T21" s="353" t="s">
         <v>1626</v>
       </c>
-      <c r="U21" s="354"/>
-      <c r="V21" s="354"/>
-      <c r="W21" s="354"/>
-      <c r="X21" s="354"/>
-      <c r="Y21" s="354"/>
-      <c r="Z21" s="354"/>
+      <c r="U21" s="353"/>
+      <c r="V21" s="353"/>
+      <c r="W21" s="353"/>
+      <c r="X21" s="353"/>
+      <c r="Y21" s="353"/>
+      <c r="Z21" s="353"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="142"/>
       <c r="B22" s="142"/>
-      <c r="C22" s="356"/>
+      <c r="C22" s="355"/>
       <c r="D22" s="142"/>
       <c r="E22" s="142"/>
       <c r="F22" s="142"/>
@@ -29308,13 +29304,13 @@
       <c r="S35" s="93" t="s">
         <v>129</v>
       </c>
-      <c r="T35" s="357"/>
-      <c r="U35" s="357"/>
-      <c r="V35" s="357"/>
-      <c r="W35" s="357"/>
-      <c r="X35" s="357"/>
-      <c r="Y35" s="357"/>
-      <c r="Z35" s="357"/>
+      <c r="T35" s="356"/>
+      <c r="U35" s="356"/>
+      <c r="V35" s="356"/>
+      <c r="W35" s="356"/>
+      <c r="X35" s="356"/>
+      <c r="Y35" s="356"/>
+      <c r="Z35" s="356"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="108" t="s">
@@ -29701,15 +29697,15 @@
       <c r="S42" s="93" t="s">
         <v>129</v>
       </c>
-      <c r="T42" s="358" t="s">
+      <c r="T42" s="357" t="s">
         <v>1658</v>
       </c>
-      <c r="U42" s="358"/>
-      <c r="V42" s="358"/>
-      <c r="W42" s="358"/>
-      <c r="X42" s="358"/>
-      <c r="Y42" s="358"/>
-      <c r="Z42" s="358"/>
+      <c r="U42" s="357"/>
+      <c r="V42" s="357"/>
+      <c r="W42" s="357"/>
+      <c r="X42" s="357"/>
+      <c r="Y42" s="357"/>
+      <c r="Z42" s="357"/>
     </row>
     <row r="43" customFormat="false" ht="52.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="108" t="s">
@@ -29916,287 +29912,287 @@
       <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="359" t="s">
+      <c r="A1" s="358" t="s">
         <v>1672</v>
       </c>
-      <c r="B1" s="360"/>
-      <c r="C1" s="360"/>
-      <c r="D1" s="360"/>
-      <c r="E1" s="360"/>
-      <c r="F1" s="360"/>
-      <c r="G1" s="360"/>
-      <c r="H1" s="360"/>
-      <c r="I1" s="360"/>
-      <c r="J1" s="360"/>
-      <c r="K1" s="360"/>
-      <c r="L1" s="360"/>
-      <c r="M1" s="360"/>
+      <c r="B1" s="359"/>
+      <c r="C1" s="359"/>
+      <c r="D1" s="359"/>
+      <c r="E1" s="359"/>
+      <c r="F1" s="359"/>
+      <c r="G1" s="359"/>
+      <c r="H1" s="359"/>
+      <c r="I1" s="359"/>
+      <c r="J1" s="359"/>
+      <c r="K1" s="359"/>
+      <c r="L1" s="359"/>
+      <c r="M1" s="359"/>
     </row>
     <row r="2" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="359" t="s">
+      <c r="A2" s="358" t="s">
         <v>1673</v>
       </c>
-      <c r="B2" s="360" t="s">
+      <c r="B2" s="359" t="s">
         <v>96</v>
       </c>
-      <c r="C2" s="360"/>
-      <c r="D2" s="360"/>
-      <c r="E2" s="360"/>
-      <c r="F2" s="360"/>
-      <c r="G2" s="360"/>
-      <c r="H2" s="360"/>
-      <c r="I2" s="360"/>
-      <c r="J2" s="360"/>
-      <c r="K2" s="360"/>
-      <c r="L2" s="360"/>
-      <c r="M2" s="360"/>
+      <c r="C2" s="359"/>
+      <c r="D2" s="359"/>
+      <c r="E2" s="359"/>
+      <c r="F2" s="359"/>
+      <c r="G2" s="359"/>
+      <c r="H2" s="359"/>
+      <c r="I2" s="359"/>
+      <c r="J2" s="359"/>
+      <c r="K2" s="359"/>
+      <c r="L2" s="359"/>
+      <c r="M2" s="359"/>
     </row>
     <row r="3" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="361" t="s">
+      <c r="A3" s="360" t="s">
         <v>1674</v>
       </c>
-      <c r="B3" s="362" t="s">
+      <c r="B3" s="361" t="s">
         <v>1675</v>
       </c>
-      <c r="C3" s="363" t="s">
+      <c r="C3" s="362" t="s">
         <v>1676</v>
       </c>
-      <c r="D3" s="364" t="s">
+      <c r="D3" s="363" t="s">
         <v>1677</v>
       </c>
-      <c r="E3" s="364" t="s">
+      <c r="E3" s="363" t="s">
         <v>1678</v>
       </c>
-      <c r="F3" s="349" t="s">
+      <c r="F3" s="348" t="s">
         <v>1679</v>
       </c>
-      <c r="G3" s="349"/>
-      <c r="H3" s="365" t="s">
+      <c r="G3" s="348"/>
+      <c r="H3" s="364" t="s">
         <v>121</v>
       </c>
-      <c r="I3" s="365"/>
-      <c r="J3" s="365"/>
-      <c r="K3" s="365"/>
-      <c r="L3" s="365"/>
-      <c r="M3" s="365"/>
+      <c r="I3" s="364"/>
+      <c r="J3" s="364"/>
+      <c r="K3" s="364"/>
+      <c r="L3" s="364"/>
+      <c r="M3" s="364"/>
     </row>
     <row r="4" customFormat="false" ht="46.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="366" t="s">
+      <c r="A4" s="365" t="s">
         <v>1680</v>
       </c>
-      <c r="B4" s="367" t="n">
+      <c r="B4" s="366" t="n">
         <v>17</v>
       </c>
-      <c r="C4" s="368" t="n">
+      <c r="C4" s="367" t="n">
         <v>56</v>
       </c>
-      <c r="D4" s="368" t="n">
+      <c r="D4" s="367" t="n">
         <v>95</v>
       </c>
-      <c r="E4" s="368" t="s">
+      <c r="E4" s="367" t="s">
         <v>1681</v>
       </c>
-      <c r="F4" s="369"/>
-      <c r="G4" s="369"/>
-      <c r="H4" s="370" t="s">
+      <c r="F4" s="368"/>
+      <c r="G4" s="368"/>
+      <c r="H4" s="369" t="s">
         <v>1682</v>
       </c>
-      <c r="I4" s="370"/>
-      <c r="J4" s="370"/>
-      <c r="K4" s="370"/>
-      <c r="L4" s="370"/>
-      <c r="M4" s="370"/>
+      <c r="I4" s="369"/>
+      <c r="J4" s="369"/>
+      <c r="K4" s="369"/>
+      <c r="L4" s="369"/>
+      <c r="M4" s="369"/>
     </row>
     <row r="5" customFormat="false" ht="46.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="371" t="s">
+      <c r="A5" s="370" t="s">
         <v>1683</v>
       </c>
-      <c r="B5" s="372" t="n">
+      <c r="B5" s="371" t="n">
         <f aca="false">(B4-17)/78</f>
         <v>0</v>
       </c>
-      <c r="C5" s="373" t="n">
+      <c r="C5" s="372" t="n">
         <f aca="false">(C4-17)/78</f>
         <v>0.5</v>
       </c>
-      <c r="D5" s="373" t="n">
+      <c r="D5" s="372" t="n">
         <f aca="false">(D4-17)/78</f>
         <v>1</v>
       </c>
-      <c r="E5" s="373" t="s">
+      <c r="E5" s="372" t="s">
         <v>1681</v>
       </c>
       <c r="F5" s="321" t="s">
         <v>1684</v>
       </c>
       <c r="G5" s="321"/>
-      <c r="H5" s="374" t="s">
+      <c r="H5" s="373" t="s">
         <v>1685</v>
       </c>
-      <c r="I5" s="374"/>
-      <c r="J5" s="374"/>
-      <c r="K5" s="374"/>
-      <c r="L5" s="374"/>
-      <c r="M5" s="374"/>
+      <c r="I5" s="373"/>
+      <c r="J5" s="373"/>
+      <c r="K5" s="373"/>
+      <c r="L5" s="373"/>
+      <c r="M5" s="373"/>
     </row>
     <row r="6" customFormat="false" ht="46.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="366" t="s">
+      <c r="A6" s="365" t="s">
         <v>1686</v>
       </c>
-      <c r="B6" s="375" t="n">
+      <c r="B6" s="374" t="n">
         <f aca="false">12+(B5*28)</f>
         <v>12</v>
       </c>
-      <c r="C6" s="376" t="n">
+      <c r="C6" s="375" t="n">
         <f aca="false">12+(C5*28)</f>
         <v>26</v>
       </c>
-      <c r="D6" s="376" t="n">
+      <c r="D6" s="375" t="n">
         <f aca="false">12+(D5*28)</f>
         <v>40</v>
       </c>
-      <c r="E6" s="376" t="n">
+      <c r="E6" s="375" t="n">
         <v>9000</v>
       </c>
-      <c r="F6" s="377" t="s">
+      <c r="F6" s="376" t="s">
         <v>1687</v>
       </c>
-      <c r="G6" s="377"/>
-      <c r="H6" s="370" t="s">
+      <c r="G6" s="376"/>
+      <c r="H6" s="369" t="s">
         <v>1688</v>
       </c>
-      <c r="I6" s="370"/>
-      <c r="J6" s="370"/>
-      <c r="K6" s="370"/>
-      <c r="L6" s="370"/>
-      <c r="M6" s="370"/>
+      <c r="I6" s="369"/>
+      <c r="J6" s="369"/>
+      <c r="K6" s="369"/>
+      <c r="L6" s="369"/>
+      <c r="M6" s="369"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="378" t="s">
+      <c r="A7" s="377" t="s">
         <v>1689</v>
       </c>
-      <c r="B7" s="379" t="n">
+      <c r="B7" s="378" t="n">
         <f aca="false">10+(B5/7)</f>
         <v>10</v>
       </c>
-      <c r="C7" s="380" t="n">
+      <c r="C7" s="379" t="n">
         <f aca="false">10+(C5/7)</f>
         <v>10.0714285714286</v>
       </c>
-      <c r="D7" s="380" t="n">
+      <c r="D7" s="379" t="n">
         <f aca="false">10+(D5/7)</f>
         <v>10.1428571428571</v>
       </c>
-      <c r="E7" s="381" t="n">
+      <c r="E7" s="380" t="n">
         <v>18</v>
       </c>
       <c r="F7" s="321" t="s">
         <v>1690</v>
       </c>
       <c r="G7" s="321"/>
-      <c r="H7" s="382" t="s">
+      <c r="H7" s="381" t="s">
         <v>1691</v>
       </c>
-      <c r="I7" s="382"/>
-      <c r="J7" s="382"/>
-      <c r="K7" s="382"/>
-      <c r="L7" s="382"/>
-      <c r="M7" s="382"/>
+      <c r="I7" s="381"/>
+      <c r="J7" s="381"/>
+      <c r="K7" s="381"/>
+      <c r="L7" s="381"/>
+      <c r="M7" s="381"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="383" t="s">
+      <c r="A8" s="382" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="375" t="n">
+      <c r="B8" s="374" t="n">
         <f aca="false">6+(B5*2)</f>
         <v>6</v>
       </c>
-      <c r="C8" s="376" t="n">
+      <c r="C8" s="375" t="n">
         <f aca="false">6+(C5*2)</f>
         <v>7</v>
       </c>
-      <c r="D8" s="376" t="n">
+      <c r="D8" s="375" t="n">
         <f aca="false">6+(D5*2)</f>
         <v>8</v>
       </c>
-      <c r="E8" s="376" t="n">
+      <c r="E8" s="375" t="n">
         <v>12</v>
       </c>
-      <c r="F8" s="377" t="s">
+      <c r="F8" s="376" t="s">
         <v>1692</v>
       </c>
-      <c r="G8" s="377"/>
-      <c r="H8" s="384" t="s">
+      <c r="G8" s="376"/>
+      <c r="H8" s="383" t="s">
         <v>1693</v>
       </c>
-      <c r="I8" s="384"/>
-      <c r="J8" s="384"/>
-      <c r="K8" s="384"/>
-      <c r="L8" s="384"/>
-      <c r="M8" s="384"/>
+      <c r="I8" s="383"/>
+      <c r="J8" s="383"/>
+      <c r="K8" s="383"/>
+      <c r="L8" s="383"/>
+      <c r="M8" s="383"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="378" t="s">
+      <c r="A9" s="377" t="s">
         <v>1694</v>
       </c>
-      <c r="B9" s="379" t="n">
+      <c r="B9" s="378" t="n">
         <f aca="false">6+(B5*0.1)</f>
         <v>6</v>
       </c>
-      <c r="C9" s="385" t="n">
+      <c r="C9" s="384" t="n">
         <f aca="false">6+(C5)</f>
         <v>6.5</v>
       </c>
-      <c r="D9" s="381" t="n">
+      <c r="D9" s="380" t="n">
         <f aca="false">6+(D5)</f>
         <v>7</v>
       </c>
-      <c r="E9" s="381" t="n">
+      <c r="E9" s="380" t="n">
         <v>8</v>
       </c>
       <c r="F9" s="321" t="s">
         <v>1695</v>
       </c>
       <c r="G9" s="321"/>
-      <c r="H9" s="382"/>
-      <c r="I9" s="382"/>
-      <c r="J9" s="382"/>
-      <c r="K9" s="382"/>
-      <c r="L9" s="382"/>
-      <c r="M9" s="382"/>
+      <c r="H9" s="381"/>
+      <c r="I9" s="381"/>
+      <c r="J9" s="381"/>
+      <c r="K9" s="381"/>
+      <c r="L9" s="381"/>
+      <c r="M9" s="381"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="386" t="s">
+      <c r="A10" s="385" t="s">
         <v>1696</v>
       </c>
-      <c r="B10" s="387" t="n">
+      <c r="B10" s="386" t="n">
         <f aca="false">(0.5+(B5*0.1))*100</f>
         <v>50</v>
       </c>
-      <c r="C10" s="388" t="n">
+      <c r="C10" s="387" t="n">
         <f aca="false">(0.5+(C5*0.1))*100</f>
         <v>55</v>
       </c>
-      <c r="D10" s="388" t="n">
+      <c r="D10" s="387" t="n">
         <f aca="false">(0.5+(D5*0.1))*100</f>
         <v>60</v>
       </c>
-      <c r="E10" s="388" t="n">
+      <c r="E10" s="387" t="n">
         <v>110</v>
       </c>
-      <c r="F10" s="389" t="s">
+      <c r="F10" s="388" t="s">
         <v>1697</v>
       </c>
-      <c r="G10" s="389"/>
-      <c r="H10" s="390"/>
-      <c r="I10" s="390"/>
-      <c r="J10" s="390"/>
-      <c r="K10" s="390"/>
-      <c r="L10" s="390"/>
-      <c r="M10" s="390"/>
+      <c r="G10" s="388"/>
+      <c r="H10" s="389"/>
+      <c r="I10" s="389"/>
+      <c r="J10" s="389"/>
+      <c r="K10" s="389"/>
+      <c r="L10" s="389"/>
+      <c r="M10" s="389"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
@@ -30316,19 +30312,19 @@
       <c r="V18" s="177" t="s">
         <v>1712</v>
       </c>
-      <c r="W18" s="391" t="s">
+      <c r="W18" s="390" t="s">
         <v>1713</v>
       </c>
-      <c r="X18" s="391"/>
-      <c r="Y18" s="391"/>
-      <c r="Z18" s="391"/>
-      <c r="AA18" s="391"/>
-      <c r="AB18" s="391"/>
-      <c r="AC18" s="392"/>
-      <c r="AD18" s="392"/>
-      <c r="AE18" s="392"/>
-      <c r="AF18" s="392"/>
-      <c r="AG18" s="392"/>
+      <c r="X18" s="390"/>
+      <c r="Y18" s="390"/>
+      <c r="Z18" s="390"/>
+      <c r="AA18" s="390"/>
+      <c r="AB18" s="390"/>
+      <c r="AC18" s="391"/>
+      <c r="AD18" s="391"/>
+      <c r="AE18" s="391"/>
+      <c r="AF18" s="391"/>
+      <c r="AG18" s="391"/>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="162" t="s">
@@ -30456,14 +30452,14 @@
       <c r="V23" s="102" t="s">
         <v>1727</v>
       </c>
-      <c r="W23" s="393" t="s">
+      <c r="W23" s="392" t="s">
         <v>92</v>
       </c>
-      <c r="X23" s="393"/>
-      <c r="Y23" s="393"/>
-      <c r="Z23" s="393"/>
-      <c r="AA23" s="393"/>
-      <c r="AB23" s="393"/>
+      <c r="X23" s="392"/>
+      <c r="Y23" s="392"/>
+      <c r="Z23" s="392"/>
+      <c r="AA23" s="392"/>
+      <c r="AB23" s="392"/>
       <c r="AC23" s="102"/>
       <c r="AD23" s="102"/>
       <c r="AE23" s="102"/>
@@ -30546,11 +30542,11 @@
       <c r="Z26" s="166"/>
       <c r="AA26" s="166"/>
       <c r="AB26" s="166"/>
-      <c r="AC26" s="344"/>
-      <c r="AD26" s="344"/>
-      <c r="AE26" s="344"/>
-      <c r="AF26" s="344"/>
-      <c r="AG26" s="344"/>
+      <c r="AC26" s="343"/>
+      <c r="AD26" s="343"/>
+      <c r="AE26" s="343"/>
+      <c r="AF26" s="343"/>
+      <c r="AG26" s="343"/>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="162" t="s">
@@ -30602,11 +30598,11 @@
       <c r="Z28" s="166"/>
       <c r="AA28" s="166"/>
       <c r="AB28" s="166"/>
-      <c r="AC28" s="344"/>
-      <c r="AD28" s="344"/>
-      <c r="AE28" s="344"/>
-      <c r="AF28" s="344"/>
-      <c r="AG28" s="344"/>
+      <c r="AC28" s="343"/>
+      <c r="AD28" s="343"/>
+      <c r="AE28" s="343"/>
+      <c r="AF28" s="343"/>
+      <c r="AG28" s="343"/>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="162" t="s">
@@ -30647,19 +30643,19 @@
       <c r="V30" s="162" t="s">
         <v>1727</v>
       </c>
-      <c r="W30" s="391" t="s">
+      <c r="W30" s="390" t="s">
         <v>677</v>
       </c>
-      <c r="X30" s="391"/>
-      <c r="Y30" s="391"/>
-      <c r="Z30" s="391"/>
-      <c r="AA30" s="391"/>
-      <c r="AB30" s="391"/>
-      <c r="AC30" s="392"/>
-      <c r="AD30" s="392"/>
-      <c r="AE30" s="392"/>
-      <c r="AF30" s="392"/>
-      <c r="AG30" s="392"/>
+      <c r="X30" s="390"/>
+      <c r="Y30" s="390"/>
+      <c r="Z30" s="390"/>
+      <c r="AA30" s="390"/>
+      <c r="AB30" s="390"/>
+      <c r="AC30" s="391"/>
+      <c r="AD30" s="391"/>
+      <c r="AE30" s="391"/>
+      <c r="AF30" s="391"/>
+      <c r="AG30" s="391"/>
     </row>
   </sheetData>
   <mergeCells count="33">
@@ -30722,9 +30718,9 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="45" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="45" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33572,7 +33568,7 @@
       <selection pane="bottomRight" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="38.43"/>
@@ -37176,7 +37172,7 @@
       <selection pane="bottomRight" activeCell="L52" activeCellId="0" sqref="L52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="21.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.625" defaultRowHeight="21.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.43"/>
@@ -40487,7 +40483,7 @@
   </sheetPr>
   <dimension ref="A1:AG1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="D16" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
@@ -40495,7 +40491,7 @@
       <selection pane="bottomRight" activeCell="I37" activeCellId="0" sqref="I37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25"/>
@@ -43132,15 +43128,15 @@
   </sheetPr>
   <dimension ref="A1:AA1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D14" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
-      <selection pane="bottomRight" activeCell="K34" activeCellId="0" sqref="K34"/>
+      <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="I14" activeCellId="0" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.14"/>
@@ -45586,7 +45582,7 @@
       <selection pane="bottomRight" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="37.86"/>
@@ -48176,7 +48172,7 @@
       <selection pane="bottomRight" activeCell="J37" activeCellId="0" sqref="J37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="43.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.29"/>

</xml_diff>